<commit_message>
read out is now functional at the individual level, added reading out of ctrl file and exp file, added to-dos
</commit_message>
<xml_diff>
--- a/resources/Screening_overview.xlsx
+++ b/resources/Screening_overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mhuismans/surfdrive/Promotie/12. STRATEGIC/Analyse 2.0/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63A9ECC5-AE5F-374C-930E-A8E04FF20C0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77D6301D-698D-614D-9D19-350A541AAD62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="340" yWindow="500" windowWidth="26840" windowHeight="15940" xr2:uid="{D8839ED9-3626-B54B-A818-DC0AE9E1EE32}"/>
   </bookViews>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="84">
-  <si>
-    <t>STR-ID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="85">
   <si>
     <t>Datum control (D0)</t>
   </si>
@@ -47,18 +44,6 @@
     <t>Datum experiment (D5)</t>
   </si>
   <si>
-    <t>Versie screeningsopzet</t>
-  </si>
-  <si>
-    <t>Organoid</t>
-  </si>
-  <si>
-    <t>Condition</t>
-  </si>
-  <si>
-    <t>Group</t>
-  </si>
-  <si>
     <t>QscoreD0</t>
   </si>
   <si>
@@ -83,9 +68,6 @@
     <t>STR01</t>
   </si>
   <si>
-    <t>FullscreenV1</t>
-  </si>
-  <si>
     <t>RAS04</t>
   </si>
   <si>
@@ -128,9 +110,6 @@
     <t>STR10</t>
   </si>
   <si>
-    <t>FullscreenV2</t>
-  </si>
-  <si>
     <t>OPT0015</t>
   </si>
   <si>
@@ -269,25 +248,49 @@
     <t>3 min later uitgelezen</t>
   </si>
   <si>
-    <t>HalfScreen</t>
-  </si>
-  <si>
-    <t>WNT normal</t>
-  </si>
-  <si>
-    <t>WNT high</t>
-  </si>
-  <si>
-    <t>WNT low</t>
-  </si>
-  <si>
-    <t>D0RowStart</t>
-  </si>
-  <si>
     <t>D0_inverted</t>
   </si>
   <si>
     <t>D5_inverted</t>
+  </si>
+  <si>
+    <t>org_id</t>
+  </si>
+  <si>
+    <t>exp_cond</t>
+  </si>
+  <si>
+    <t>org_name</t>
+  </si>
+  <si>
+    <t>WNT_high</t>
+  </si>
+  <si>
+    <t>WNT_low</t>
+  </si>
+  <si>
+    <t>screen_setup</t>
+  </si>
+  <si>
+    <t>chemo_naive</t>
+  </si>
+  <si>
+    <t>RASTRIC</t>
+  </si>
+  <si>
+    <t>STR_ID</t>
+  </si>
+  <si>
+    <t>D0_rowstart</t>
+  </si>
+  <si>
+    <t>FullscreenV1.xlsx</t>
+  </si>
+  <si>
+    <t>FullscreenV2.xlsx</t>
+  </si>
+  <si>
+    <t>HalfScreen.xlsx</t>
   </si>
 </sst>
 </file>
@@ -409,7 +412,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -427,12 +430,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -748,86 +747,97 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{475CD61C-36C8-3749-9107-2737F390B1D4}">
-  <dimension ref="A1:S43"/>
+  <dimension ref="A1:U43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="5" ySplit="1" topLeftCell="F19" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.1640625" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.33203125" customWidth="1"/>
-    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11" customWidth="1"/>
-    <col min="12" max="12" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="42.6640625" customWidth="1"/>
-    <col min="16" max="16" width="23.83203125" customWidth="1"/>
-    <col min="17" max="17" width="17.33203125" customWidth="1"/>
-    <col min="19" max="19" width="23.5" customWidth="1"/>
+    <col min="7" max="7" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.33203125" customWidth="1"/>
+    <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11" customWidth="1"/>
+    <col min="14" max="14" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="42.6640625" customWidth="1"/>
+    <col min="18" max="18" width="23.83203125" customWidth="1"/>
+    <col min="19" max="19" width="17.33203125" customWidth="1"/>
+    <col min="21" max="21" width="23.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="R1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="S1" s="2"/>
+      <c r="T1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="L1" s="1" t="s">
+      <c r="U1" s="13"/>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>9</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O1" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="S1" s="14"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>14</v>
       </c>
       <c r="B2" s="3">
         <v>44670</v>
@@ -836,34 +846,44 @@
         <v>44675</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>82</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="G2" t="str">
-        <f>IF(LEFT(E2,3)="RAS","RASTRIC","OPTIC")</f>
-        <v>RASTRIC</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2" t="s">
-        <v>17</v>
-      </c>
-      <c r="N2" t="s">
-        <v>18</v>
-      </c>
-      <c r="R2" s="4">
-        <v>0</v>
-      </c>
-      <c r="S2" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+        <f>IF(ISBLANK(F2),E2,E2&amp;"_"&amp;F2)</f>
+        <v>RAS04</v>
+      </c>
+      <c r="H2">
+        <f>IF(LEFT(E2,3)="RAS",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2" t="s">
+        <v>11</v>
+      </c>
+      <c r="P2" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="T2" s="4">
+        <v>0</v>
+      </c>
+      <c r="U2" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B3" s="3">
         <v>44670</v>
@@ -872,27 +892,37 @@
         <v>44675</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>82</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="G3" t="str">
-        <f t="shared" ref="G3:G43" si="0">IF(LEFT(E3,3)="RAS","RASTRIC","OPTIC")</f>
-        <v>OPTIC</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="M3" t="s">
-        <v>17</v>
-      </c>
-      <c r="R3" s="4"/>
-      <c r="S3" s="5"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+        <f t="shared" ref="G3:G43" si="0">IF(ISBLANK(F3),E3,E3&amp;"_"&amp;F3)</f>
+        <v>OPT0112</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H43" si="1">IF(LEFT(E3,3)="RAS",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="T3" s="4"/>
+      <c r="U3" s="5"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3">
         <v>44670</v>
@@ -901,27 +931,37 @@
         <v>44675</v>
       </c>
       <c r="D4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E4" t="s">
         <v>15</v>
       </c>
-      <c r="E4" t="s">
-        <v>21</v>
-      </c>
       <c r="G4" t="str">
         <f t="shared" si="0"/>
-        <v>OPTIC</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4" t="s">
-        <v>17</v>
-      </c>
-      <c r="R4" s="4"/>
-      <c r="S4" s="5"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+        <v>OPT0016</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="T4" s="4"/>
+      <c r="U4" s="5"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B5" s="3">
         <v>44679</v>
@@ -930,34 +970,44 @@
         <v>44683</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>82</v>
       </c>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="G5" t="str">
         <f t="shared" si="0"/>
-        <v>RASTRIC</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-      <c r="M5" t="s">
-        <v>17</v>
-      </c>
-      <c r="N5" t="s">
+        <v>RAS25</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5" t="s">
+        <v>11</v>
+      </c>
+      <c r="P5" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="T5" s="4">
+        <v>1</v>
+      </c>
+      <c r="U5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="R5" s="4">
-        <v>1</v>
-      </c>
-      <c r="S5" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B6" s="3">
         <v>44679</v>
@@ -966,27 +1016,37 @@
         <v>44683</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>82</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" si="0"/>
-        <v>OPTIC</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-      <c r="M6" t="s">
-        <v>17</v>
-      </c>
-      <c r="R6" s="4"/>
-      <c r="S6" s="5"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+        <v>OPT0014</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="T6" s="4"/>
+      <c r="U6" s="5"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B7" s="3">
         <v>44706</v>
@@ -995,34 +1055,44 @@
         <v>44711</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>82</v>
       </c>
       <c r="E7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" si="0"/>
-        <v>RASTRIC</v>
-      </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
-      <c r="M7" t="s">
-        <v>17</v>
-      </c>
-      <c r="N7" t="s">
-        <v>18</v>
-      </c>
-      <c r="R7" s="4">
-        <v>2</v>
-      </c>
-      <c r="S7" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+        <v>RAS21</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7" t="s">
+        <v>11</v>
+      </c>
+      <c r="P7" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="T7" s="4">
+        <v>2</v>
+      </c>
+      <c r="U7" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B8" s="3">
         <v>44741</v>
@@ -1031,34 +1101,44 @@
         <v>44746</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="E8" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="G8" t="str">
         <f t="shared" si="0"/>
-        <v>OPTIC</v>
-      </c>
-      <c r="L8">
-        <v>2</v>
-      </c>
-      <c r="M8" t="s">
-        <v>17</v>
-      </c>
-      <c r="N8" t="s">
-        <v>32</v>
-      </c>
-      <c r="R8" s="6">
+        <v>OPT0015</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>2</v>
+      </c>
+      <c r="O8" t="s">
+        <v>11</v>
+      </c>
+      <c r="P8" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="T8" s="6">
         <v>3</v>
       </c>
-      <c r="S8" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="U8" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B9" s="3">
         <v>44741</v>
@@ -1067,31 +1147,41 @@
         <v>44746</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="E9" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="G9" t="str">
         <f t="shared" si="0"/>
-        <v>RASTRIC</v>
-      </c>
-      <c r="L9">
+        <v>RAS04</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="N9">
         <v>3</v>
       </c>
-      <c r="M9" t="s">
-        <v>17</v>
-      </c>
-      <c r="R9" s="6">
+      <c r="O9" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="T9" s="6">
         <v>3</v>
       </c>
-      <c r="S9" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="U9" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B10" s="3">
         <v>44750</v>
@@ -1100,25 +1190,35 @@
         <v>44755</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="E10" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G10" t="str">
         <f t="shared" si="0"/>
-        <v>OPTIC</v>
-      </c>
-      <c r="L10">
+        <v>OPT0016</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="N10">
         <v>3</v>
       </c>
-      <c r="M10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="O10" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B11" s="3">
         <v>44750</v>
@@ -1127,25 +1227,35 @@
         <v>44755</v>
       </c>
       <c r="D11" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="E11" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="G11" t="str">
         <f t="shared" si="0"/>
-        <v>RASTRIC</v>
-      </c>
-      <c r="L11">
+        <v>RAS25</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="N11">
         <v>3</v>
       </c>
-      <c r="M11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="O11" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B12" s="3">
         <v>44750</v>
@@ -1154,25 +1264,35 @@
         <v>44755</v>
       </c>
       <c r="D12" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="E12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="G12" t="str">
         <f t="shared" si="0"/>
-        <v>OPTIC</v>
-      </c>
-      <c r="L12">
+        <v>OPT0112</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="N12">
         <v>3</v>
       </c>
-      <c r="M12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="O12" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B13" s="3">
         <v>44760</v>
@@ -1181,25 +1301,35 @@
         <v>44765</v>
       </c>
       <c r="D13" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="E13" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="G13" t="str">
         <f t="shared" si="0"/>
-        <v>RASTRIC</v>
-      </c>
-      <c r="L13">
+        <v>RAS21</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="N13">
         <v>3</v>
       </c>
-      <c r="M13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="O13" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B14" s="3">
         <v>44760</v>
@@ -1208,25 +1338,35 @@
         <v>44765</v>
       </c>
       <c r="D14" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="E14" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="G14" t="str">
         <f t="shared" si="0"/>
-        <v>OPTIC</v>
-      </c>
-      <c r="L14">
+        <v>OPT0014</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="N14">
         <v>3</v>
       </c>
-      <c r="M14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="O14" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B15" s="3">
         <v>44771</v>
@@ -1235,28 +1375,44 @@
         <v>44776</v>
       </c>
       <c r="D15" t="s">
+        <v>83</v>
+      </c>
+      <c r="E15" t="s">
         <v>30</v>
       </c>
-      <c r="E15" t="s">
-        <v>37</v>
-      </c>
       <c r="G15" t="str">
         <f t="shared" si="0"/>
-        <v>OPTIC</v>
+        <v>OPT0005</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
       </c>
       <c r="L15">
-        <v>2</v>
-      </c>
-      <c r="M15" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="N15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+      <c r="M15">
+        <v>1</v>
+      </c>
+      <c r="N15">
+        <v>2</v>
+      </c>
+      <c r="O15" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="P15" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B16" s="3">
         <v>44771</v>
@@ -1265,29 +1421,45 @@
         <v>44776</v>
       </c>
       <c r="D16" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="F16" s="9"/>
       <c r="G16" t="str">
         <f t="shared" si="0"/>
-        <v>OPTIC</v>
-      </c>
-      <c r="L16" s="10">
-        <v>1</v>
-      </c>
-      <c r="M16" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="N16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+        <v>HUB-02-C2-89</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="L16">
+        <v>13</v>
+      </c>
+      <c r="M16">
+        <v>1</v>
+      </c>
+      <c r="N16" s="10">
+        <v>1</v>
+      </c>
+      <c r="O16" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="P16" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B17" s="3">
         <v>44798</v>
@@ -1296,28 +1468,44 @@
         <v>44803</v>
       </c>
       <c r="D17" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="E17" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="G17" t="str">
         <f t="shared" si="0"/>
-        <v>RASTRIC</v>
+        <v>RAS12</v>
       </c>
       <c r="H17">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
         <v>3</v>
       </c>
-      <c r="L17" s="11">
-        <v>2</v>
-      </c>
-      <c r="M17" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="L17">
+        <v>13</v>
+      </c>
+      <c r="M17">
+        <v>1</v>
+      </c>
+      <c r="N17" s="11">
+        <v>2</v>
+      </c>
+      <c r="O17" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B18" s="3">
         <v>44798</v>
@@ -1326,32 +1514,48 @@
         <v>44803</v>
       </c>
       <c r="D18" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="F18" s="9"/>
       <c r="G18" t="str">
         <f t="shared" si="0"/>
-        <v>RASTRIC</v>
+        <v>RAS27</v>
       </c>
       <c r="H18">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
         <v>3</v>
       </c>
-      <c r="L18" s="11">
-        <v>2</v>
-      </c>
-      <c r="M18" t="s">
-        <v>17</v>
-      </c>
-      <c r="N18" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="L18">
+        <v>15</v>
+      </c>
+      <c r="M18">
+        <v>1</v>
+      </c>
+      <c r="N18" s="11">
+        <v>2</v>
+      </c>
+      <c r="O18" t="s">
+        <v>11</v>
+      </c>
+      <c r="P18" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B19" s="3">
         <v>44798</v>
@@ -1360,35 +1564,51 @@
         <v>44803</v>
       </c>
       <c r="D19" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="F19" s="9"/>
       <c r="G19" t="str">
         <f t="shared" si="0"/>
-        <v>OPTIC</v>
+        <v>OPT0413</v>
       </c>
       <c r="H19">
-        <v>2</v>
-      </c>
-      <c r="I19" t="s">
-        <v>47</v>
-      </c>
-      <c r="L19" s="11">
-        <v>2</v>
-      </c>
-      <c r="M19" t="s">
-        <v>17</v>
-      </c>
-      <c r="N19" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="J19">
+        <v>2</v>
+      </c>
+      <c r="K19" t="s">
+        <v>40</v>
+      </c>
+      <c r="L19">
+        <v>1</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19" s="11">
+        <v>2</v>
+      </c>
+      <c r="O19" t="s">
+        <v>11</v>
+      </c>
+      <c r="P19" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B20" s="3">
         <v>44823</v>
@@ -1397,34 +1617,50 @@
         <v>44828</v>
       </c>
       <c r="D20" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="E20" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="G20" t="str">
         <f t="shared" si="0"/>
-        <v>RASTRIC</v>
+        <v>RAS05</v>
       </c>
       <c r="H20">
-        <v>2</v>
-      </c>
-      <c r="L20" s="11">
-        <v>2</v>
-      </c>
-      <c r="M20" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="N20" t="s">
-        <v>50</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>2</v>
+      </c>
+      <c r="L20">
+        <v>9</v>
+      </c>
+      <c r="M20">
+        <v>1</v>
+      </c>
+      <c r="N20" s="11">
+        <v>2</v>
+      </c>
+      <c r="O20" s="12" t="s">
+        <v>11</v>
       </c>
       <c r="P20" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
+      <c r="R20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B21" s="3">
         <v>44823</v>
@@ -1433,34 +1669,50 @@
         <v>44828</v>
       </c>
       <c r="D21" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="E21" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="G21" t="str">
         <f t="shared" si="0"/>
-        <v>OPTIC</v>
+        <v>OPT0419</v>
       </c>
       <c r="H21">
-        <v>2</v>
-      </c>
-      <c r="L21" s="11">
-        <v>2</v>
-      </c>
-      <c r="M21" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="N21" t="s">
-        <v>50</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>1</v>
+      </c>
+      <c r="J21">
+        <v>2</v>
+      </c>
+      <c r="L21">
+        <v>7</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21" s="11">
+        <v>2</v>
+      </c>
+      <c r="O21" s="12" t="s">
+        <v>11</v>
       </c>
       <c r="P21" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
+      <c r="R21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B22" s="3">
         <v>44830</v>
@@ -1469,31 +1721,47 @@
         <v>44835</v>
       </c>
       <c r="D22" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="E22" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="G22" t="str">
         <f t="shared" si="0"/>
-        <v>RASTRIC</v>
+        <v>RAS06</v>
       </c>
       <c r="H22">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
         <v>3</v>
       </c>
-      <c r="L22" s="11">
-        <v>2</v>
-      </c>
-      <c r="M22" t="s">
-        <v>17</v>
-      </c>
-      <c r="N22" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="L22">
+        <v>3</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22" s="11">
+        <v>2</v>
+      </c>
+      <c r="O22" t="s">
+        <v>11</v>
+      </c>
+      <c r="P22" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B23" s="3">
         <v>44830</v>
@@ -1502,31 +1770,47 @@
         <v>44835</v>
       </c>
       <c r="D23" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="E23" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="G23" t="str">
         <f t="shared" si="0"/>
-        <v>RASTRIC</v>
+        <v>RAS13</v>
       </c>
       <c r="H23">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
         <v>3</v>
       </c>
-      <c r="L23" s="11">
-        <v>2</v>
-      </c>
-      <c r="M23" t="s">
-        <v>17</v>
-      </c>
-      <c r="N23" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="L23">
+        <v>1</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="N23" s="11">
+        <v>2</v>
+      </c>
+      <c r="O23" t="s">
+        <v>11</v>
+      </c>
+      <c r="P23" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B24" s="3">
         <v>44830</v>
@@ -1535,31 +1819,47 @@
         <v>44835</v>
       </c>
       <c r="D24" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="E24" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="G24" t="str">
         <f t="shared" si="0"/>
-        <v>OPTIC</v>
+        <v>OPT0408</v>
       </c>
       <c r="H24">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+      <c r="J24">
         <v>3</v>
       </c>
-      <c r="L24" s="11">
-        <v>2</v>
-      </c>
-      <c r="M24" t="s">
-        <v>17</v>
-      </c>
-      <c r="N24" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="L24">
+        <v>5</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24" s="11">
+        <v>2</v>
+      </c>
+      <c r="O24" t="s">
+        <v>11</v>
+      </c>
+      <c r="P24" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B25" s="3">
         <v>44841</v>
@@ -1568,35 +1868,51 @@
         <v>44845</v>
       </c>
       <c r="D25" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="F25" s="9"/>
       <c r="G25" t="str">
         <f t="shared" si="0"/>
-        <v>OPTIC</v>
+        <v>OPT0034</v>
       </c>
       <c r="H25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>1</v>
+      </c>
+      <c r="J25">
         <v>3</v>
       </c>
-      <c r="I25" t="s">
-        <v>60</v>
-      </c>
-      <c r="L25" s="10">
-        <v>1</v>
-      </c>
-      <c r="M25" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="N25" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="K25" t="s">
+        <v>53</v>
+      </c>
+      <c r="L25">
+        <v>7</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
+      <c r="N25" s="10">
+        <v>1</v>
+      </c>
+      <c r="O25" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="P25" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B26" s="3">
         <v>44841</v>
@@ -1605,35 +1921,51 @@
         <v>44845</v>
       </c>
       <c r="D26" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="F26" s="9"/>
       <c r="G26" t="str">
         <f t="shared" si="0"/>
-        <v>RASTRIC</v>
+        <v>RAS11</v>
       </c>
       <c r="H26">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
         <v>3</v>
       </c>
-      <c r="I26" t="s">
-        <v>60</v>
-      </c>
-      <c r="L26" s="10">
-        <v>1</v>
-      </c>
-      <c r="M26" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="N26" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="K26" t="s">
+        <v>53</v>
+      </c>
+      <c r="L26">
+        <v>9</v>
+      </c>
+      <c r="M26">
+        <v>1</v>
+      </c>
+      <c r="N26" s="10">
+        <v>1</v>
+      </c>
+      <c r="O26" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="P26" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B27" s="3">
         <v>44862</v>
@@ -1642,34 +1974,50 @@
         <v>44867</v>
       </c>
       <c r="D27" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="E27" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="G27" t="str">
         <f t="shared" si="0"/>
-        <v>OPTIC</v>
+        <v>OPT0402</v>
       </c>
       <c r="H27">
-        <v>2</v>
-      </c>
-      <c r="I27" t="s">
-        <v>47</v>
-      </c>
-      <c r="L27" s="10">
-        <v>1</v>
-      </c>
-      <c r="M27" t="s">
-        <v>17</v>
-      </c>
-      <c r="N27" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>1</v>
+      </c>
+      <c r="J27">
+        <v>2</v>
+      </c>
+      <c r="K27" t="s">
+        <v>40</v>
+      </c>
+      <c r="L27">
+        <v>11</v>
+      </c>
+      <c r="M27">
+        <v>1</v>
+      </c>
+      <c r="N27" s="10">
+        <v>1</v>
+      </c>
+      <c r="O27" t="s">
+        <v>11</v>
+      </c>
+      <c r="P27" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B28" s="3">
         <v>44862</v>
@@ -1678,35 +2026,51 @@
         <v>44867</v>
       </c>
       <c r="D28" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="F28" s="11"/>
       <c r="G28" t="str">
         <f t="shared" si="0"/>
-        <v>RASTRIC</v>
+        <v>RAS16</v>
       </c>
       <c r="H28">
-        <v>2</v>
-      </c>
-      <c r="I28" t="s">
-        <v>47</v>
-      </c>
-      <c r="L28" s="10">
-        <v>1</v>
-      </c>
-      <c r="M28" t="s">
-        <v>17</v>
-      </c>
-      <c r="N28" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>2</v>
+      </c>
+      <c r="K28" t="s">
+        <v>40</v>
+      </c>
+      <c r="L28">
+        <v>13</v>
+      </c>
+      <c r="M28">
+        <v>1</v>
+      </c>
+      <c r="N28" s="10">
+        <v>1</v>
+      </c>
+      <c r="O28" t="s">
+        <v>11</v>
+      </c>
+      <c r="P28" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B29" s="3">
         <v>44862</v>
@@ -1715,35 +2079,51 @@
         <v>44867</v>
       </c>
       <c r="D29" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="F29" s="11"/>
       <c r="G29" t="str">
         <f t="shared" si="0"/>
-        <v>RASTRIC</v>
+        <v>RAS22</v>
       </c>
       <c r="H29">
-        <v>2</v>
-      </c>
-      <c r="I29" t="s">
-        <v>47</v>
-      </c>
-      <c r="L29" s="10">
-        <v>1</v>
-      </c>
-      <c r="M29" t="s">
-        <v>17</v>
-      </c>
-      <c r="N29" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <v>2</v>
+      </c>
+      <c r="K29" t="s">
+        <v>40</v>
+      </c>
+      <c r="L29">
+        <v>11</v>
+      </c>
+      <c r="M29">
+        <v>1</v>
+      </c>
+      <c r="N29" s="10">
+        <v>1</v>
+      </c>
+      <c r="O29" t="s">
+        <v>11</v>
+      </c>
+      <c r="P29" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B30" s="3">
         <v>44862</v>
@@ -1752,35 +2132,51 @@
         <v>44867</v>
       </c>
       <c r="D30" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="F30" s="11"/>
       <c r="G30" t="str">
         <f t="shared" si="0"/>
-        <v>RASTRIC</v>
+        <v>RAS24</v>
       </c>
       <c r="H30">
-        <v>2</v>
-      </c>
-      <c r="I30" t="s">
-        <v>47</v>
-      </c>
-      <c r="L30" s="10">
-        <v>1</v>
-      </c>
-      <c r="M30" t="s">
-        <v>17</v>
-      </c>
-      <c r="N30" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+      <c r="J30">
+        <v>2</v>
+      </c>
+      <c r="K30" t="s">
+        <v>40</v>
+      </c>
+      <c r="L30">
+        <v>9</v>
+      </c>
+      <c r="M30">
+        <v>1</v>
+      </c>
+      <c r="N30" s="10">
+        <v>1</v>
+      </c>
+      <c r="O30" t="s">
+        <v>11</v>
+      </c>
+      <c r="P30" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B31" s="3">
         <v>44911</v>
@@ -1789,31 +2185,41 @@
         <v>44916</v>
       </c>
       <c r="D31" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="E31" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="G31" t="str">
         <f t="shared" si="0"/>
-        <v>OPTIC</v>
+        <v>OPT0024</v>
       </c>
       <c r="H31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>1</v>
+      </c>
+      <c r="J31">
         <v>3</v>
       </c>
-      <c r="L31" s="11">
-        <v>2</v>
-      </c>
-      <c r="M31" t="s">
-        <v>17</v>
-      </c>
-      <c r="N31" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="N31" s="11">
+        <v>2</v>
+      </c>
+      <c r="O31" t="s">
+        <v>11</v>
+      </c>
+      <c r="P31" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B32" s="3">
         <v>44911</v>
@@ -1822,31 +2228,41 @@
         <v>44916</v>
       </c>
       <c r="D32" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="E32" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="G32" t="str">
         <f t="shared" si="0"/>
-        <v>OPTIC</v>
+        <v>OPT0030</v>
       </c>
       <c r="H32">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
+      <c r="J32">
         <v>3</v>
       </c>
-      <c r="L32" s="11">
-        <v>2</v>
-      </c>
-      <c r="M32" t="s">
-        <v>17</v>
-      </c>
-      <c r="N32" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N32" s="11">
+        <v>2</v>
+      </c>
+      <c r="O32" t="s">
+        <v>11</v>
+      </c>
+      <c r="P32" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B33" s="3">
         <v>44911</v>
@@ -1855,31 +2271,41 @@
         <v>44916</v>
       </c>
       <c r="D33" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="E33" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="G33" t="str">
         <f t="shared" si="0"/>
-        <v>OPTIC</v>
+        <v>OPT0424</v>
       </c>
       <c r="H33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+      <c r="J33">
         <v>3</v>
       </c>
-      <c r="L33" s="11">
-        <v>2</v>
-      </c>
-      <c r="M33" t="s">
-        <v>17</v>
-      </c>
-      <c r="N33" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N33" s="11">
+        <v>2</v>
+      </c>
+      <c r="O33" t="s">
+        <v>11</v>
+      </c>
+      <c r="P33" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B34" s="3">
         <v>44932</v>
@@ -1888,22 +2314,32 @@
         <v>44937</v>
       </c>
       <c r="D34" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="E34" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="G34" t="str">
         <f t="shared" si="0"/>
-        <v>OPTIC</v>
+        <v>OPT0039</v>
       </c>
       <c r="H34">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <v>1</v>
+      </c>
+      <c r="J34">
         <v>3</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B35" s="3">
         <v>44932</v>
@@ -1912,25 +2348,35 @@
         <v>44937</v>
       </c>
       <c r="D35" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="E35" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="G35" t="str">
         <f t="shared" si="0"/>
-        <v>OPTIC</v>
+        <v>OPT0024</v>
       </c>
       <c r="H35">
-        <v>2</v>
-      </c>
-      <c r="I35" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <v>1</v>
+      </c>
+      <c r="J35">
+        <v>2</v>
+      </c>
+      <c r="K35" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B36" s="3">
         <v>44932</v>
@@ -1939,25 +2385,35 @@
         <v>44937</v>
       </c>
       <c r="D36" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="E36" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="G36" t="str">
         <f t="shared" si="0"/>
-        <v>OPTIC</v>
+        <v>OPT0424</v>
       </c>
       <c r="H36">
-        <v>2</v>
-      </c>
-      <c r="I36" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <v>0</v>
+      </c>
+      <c r="J36">
+        <v>2</v>
+      </c>
+      <c r="K36" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B37" s="3">
         <v>44932</v>
@@ -1966,25 +2422,32 @@
         <v>44937</v>
       </c>
       <c r="D37" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="E37" t="s">
-        <v>72</v>
-      </c>
-      <c r="F37" s="13" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="G37" t="str">
         <f t="shared" si="0"/>
-        <v>OPTIC</v>
+        <v>OPT0030</v>
       </c>
       <c r="H37">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I37">
+        <v>0</v>
+      </c>
+      <c r="J37">
         <v>3</v>
       </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B38" s="3">
         <v>44932</v>
@@ -1993,25 +2456,35 @@
         <v>44937</v>
       </c>
       <c r="D38" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="E38" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="F38" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G38" t="str">
         <f t="shared" si="0"/>
-        <v>OPTIC</v>
+        <v>OPT0030_WNT_high</v>
       </c>
       <c r="H38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <v>0</v>
+      </c>
+      <c r="J38">
         <v>3</v>
       </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B39" s="3">
         <v>44932</v>
@@ -2020,25 +2493,35 @@
         <v>44937</v>
       </c>
       <c r="D39" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="E39" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="F39" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="G39" t="str">
         <f t="shared" si="0"/>
-        <v>OPTIC</v>
+        <v>OPT0030_WNT_low</v>
       </c>
       <c r="H39">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I39">
+        <v>0</v>
+      </c>
+      <c r="J39">
         <v>3</v>
       </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B40" s="3">
         <v>44932</v>
@@ -2047,28 +2530,38 @@
         <v>44937</v>
       </c>
       <c r="D40" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="E40" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="F40" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G40" t="str">
         <f t="shared" si="0"/>
-        <v>OPTIC</v>
+        <v>OPT0024_WNT_high</v>
       </c>
       <c r="H40">
-        <v>2</v>
-      </c>
-      <c r="I40" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <v>1</v>
+      </c>
+      <c r="J40">
+        <v>2</v>
+      </c>
+      <c r="K40" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B41" s="3">
         <v>44932</v>
@@ -2077,28 +2570,38 @@
         <v>44937</v>
       </c>
       <c r="D41" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="E41" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="F41" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="G41" t="str">
         <f t="shared" si="0"/>
-        <v>OPTIC</v>
+        <v>OPT0024_WNT_low</v>
       </c>
       <c r="H41">
-        <v>2</v>
-      </c>
-      <c r="I41" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I41">
+        <v>1</v>
+      </c>
+      <c r="J41">
+        <v>2</v>
+      </c>
+      <c r="K41" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B42" s="3">
         <v>44932</v>
@@ -2107,28 +2610,38 @@
         <v>44937</v>
       </c>
       <c r="D42" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="E42" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="F42" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G42" t="str">
         <f t="shared" si="0"/>
-        <v>OPTIC</v>
+        <v>OPT0424_WNT_high</v>
       </c>
       <c r="H42">
-        <v>2</v>
-      </c>
-      <c r="I42" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I42">
+        <v>0</v>
+      </c>
+      <c r="J42">
+        <v>2</v>
+      </c>
+      <c r="K42" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B43" s="3">
         <v>44932</v>
@@ -2137,28 +2650,38 @@
         <v>44937</v>
       </c>
       <c r="D43" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="E43" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="F43" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="G43" t="str">
         <f t="shared" si="0"/>
-        <v>OPTIC</v>
+        <v>OPT0424_WNT_low</v>
       </c>
       <c r="H43">
-        <v>2</v>
-      </c>
-      <c r="I43" t="s">
-        <v>76</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I43">
+        <v>0</v>
+      </c>
+      <c r="J43">
+        <v>2</v>
+      </c>
+      <c r="K43" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q43">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="T1:U1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Werkende code om van raw files via overzicht een overzicht te maken per organoid en op te slaan als excel
</commit_message>
<xml_diff>
--- a/resources/Screening_overview.xlsx
+++ b/resources/Screening_overview.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mhuismans/surfdrive/Promotie/12. STRATEGIC/Analyse 2.0/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77D6301D-698D-614D-9D19-350A541AAD62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4DED5FA-0C36-3D4E-9F2B-465319C4DFCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="500" windowWidth="26840" windowHeight="15940" xr2:uid="{D8839ED9-3626-B54B-A818-DC0AE9E1EE32}"/>
+    <workbookView xWindow="80" yWindow="500" windowWidth="26840" windowHeight="15940" xr2:uid="{D8839ED9-3626-B54B-A818-DC0AE9E1EE32}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,12 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="85">
   <si>
-    <t>Datum control (D0)</t>
-  </si>
-  <si>
-    <t>Datum experiment (D5)</t>
-  </si>
-  <si>
     <t>QscoreD0</t>
   </si>
   <si>
@@ -291,6 +285,12 @@
   </si>
   <si>
     <t>HalfScreen.xlsx</t>
+  </si>
+  <si>
+    <t>Date_D0</t>
+  </si>
+  <si>
+    <t>Date_D5</t>
   </si>
 </sst>
 </file>
@@ -451,7 +451,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -739,7 +739,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -750,10 +750,10 @@
   <dimension ref="A1:U43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomRight" activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -761,7 +761,8 @@
     <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.1640625" customWidth="1"/>
     <col min="4" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" customWidth="1"/>
+    <col min="6" max="6" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="22.33203125" customWidth="1"/>
@@ -776,68 +777,68 @@
   <sheetData>
     <row r="1" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>84</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="R1" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>7</v>
       </c>
       <c r="S1" s="2"/>
       <c r="T1" s="13" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="U1" s="13"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B2" s="3">
         <v>44670</v>
@@ -846,10 +847,10 @@
         <v>44675</v>
       </c>
       <c r="D2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G2" t="str">
         <f>IF(ISBLANK(F2),E2,E2&amp;"_"&amp;F2)</f>
@@ -866,24 +867,24 @@
         <v>0</v>
       </c>
       <c r="O2" t="s">
+        <v>9</v>
+      </c>
+      <c r="P2" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="T2" s="4">
+        <v>0</v>
+      </c>
+      <c r="U2" s="5" t="s">
         <v>11</v>
-      </c>
-      <c r="P2" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="T2" s="4">
-        <v>0</v>
-      </c>
-      <c r="U2" s="5" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B3" s="3">
         <v>44670</v>
@@ -892,10 +893,10 @@
         <v>44675</v>
       </c>
       <c r="D3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G3" t="str">
         <f t="shared" ref="G3:G43" si="0">IF(ISBLANK(F3),E3,E3&amp;"_"&amp;F3)</f>
@@ -912,7 +913,7 @@
         <v>0</v>
       </c>
       <c r="O3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -922,7 +923,7 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" s="3">
         <v>44670</v>
@@ -931,10 +932,10 @@
         <v>44675</v>
       </c>
       <c r="D4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G4" t="str">
         <f t="shared" si="0"/>
@@ -951,7 +952,7 @@
         <v>0</v>
       </c>
       <c r="O4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="Q4">
         <v>0</v>
@@ -961,7 +962,7 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B5" s="3">
         <v>44679</v>
@@ -970,10 +971,10 @@
         <v>44683</v>
       </c>
       <c r="D5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G5" t="str">
         <f t="shared" si="0"/>
@@ -990,10 +991,10 @@
         <v>0</v>
       </c>
       <c r="O5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="P5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="Q5">
         <v>0</v>
@@ -1002,12 +1003,12 @@
         <v>1</v>
       </c>
       <c r="U5" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B6" s="3">
         <v>44679</v>
@@ -1016,10 +1017,10 @@
         <v>44683</v>
       </c>
       <c r="D6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" si="0"/>
@@ -1036,7 +1037,7 @@
         <v>0</v>
       </c>
       <c r="O6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="Q6">
         <v>0</v>
@@ -1046,7 +1047,7 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B7" s="3">
         <v>44706</v>
@@ -1055,10 +1056,10 @@
         <v>44711</v>
       </c>
       <c r="D7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" si="0"/>
@@ -1075,10 +1076,10 @@
         <v>0</v>
       </c>
       <c r="O7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="P7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="Q7">
         <v>0</v>
@@ -1087,12 +1088,12 @@
         <v>2</v>
       </c>
       <c r="U7" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B8" s="3">
         <v>44741</v>
@@ -1101,10 +1102,10 @@
         <v>44746</v>
       </c>
       <c r="D8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G8" t="str">
         <f t="shared" si="0"/>
@@ -1116,15 +1117,21 @@
       </c>
       <c r="I8">
         <v>1</v>
+      </c>
+      <c r="L8">
+        <v>3</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
       </c>
       <c r="N8">
         <v>2</v>
       </c>
       <c r="O8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="P8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="Q8">
         <v>0</v>
@@ -1133,12 +1140,12 @@
         <v>3</v>
       </c>
       <c r="U8" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B9" s="3">
         <v>44741</v>
@@ -1147,10 +1154,10 @@
         <v>44746</v>
       </c>
       <c r="D9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G9" t="str">
         <f t="shared" si="0"/>
@@ -1162,12 +1169,18 @@
       </c>
       <c r="I9">
         <v>0</v>
+      </c>
+      <c r="L9">
+        <v>13</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
       </c>
       <c r="N9">
         <v>3</v>
       </c>
       <c r="O9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="Q9">
         <v>0</v>
@@ -1176,12 +1189,12 @@
         <v>3</v>
       </c>
       <c r="U9" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B10" s="3">
         <v>44750</v>
@@ -1190,10 +1203,10 @@
         <v>44755</v>
       </c>
       <c r="D10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G10" t="str">
         <f t="shared" si="0"/>
@@ -1204,13 +1217,19 @@
         <v>0</v>
       </c>
       <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <v>13</v>
+      </c>
+      <c r="M10">
         <v>1</v>
       </c>
       <c r="N10">
         <v>3</v>
       </c>
       <c r="O10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="Q10">
         <v>0</v>
@@ -1218,7 +1237,7 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B11" s="3">
         <v>44750</v>
@@ -1227,10 +1246,10 @@
         <v>44755</v>
       </c>
       <c r="D11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G11" t="str">
         <f t="shared" si="0"/>
@@ -1241,13 +1260,19 @@
         <v>1</v>
       </c>
       <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>3</v>
+      </c>
+      <c r="M11">
         <v>0</v>
       </c>
       <c r="N11">
         <v>3</v>
       </c>
       <c r="O11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="Q11">
         <v>0</v>
@@ -1255,7 +1280,7 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B12" s="3">
         <v>44750</v>
@@ -1264,10 +1289,10 @@
         <v>44755</v>
       </c>
       <c r="D12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G12" t="str">
         <f t="shared" si="0"/>
@@ -1279,12 +1304,18 @@
       </c>
       <c r="I12">
         <v>1</v>
+      </c>
+      <c r="L12">
+        <v>7</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
       </c>
       <c r="N12">
         <v>3</v>
       </c>
       <c r="O12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="Q12">
         <v>0</v>
@@ -1292,7 +1323,7 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B13" s="3">
         <v>44760</v>
@@ -1301,10 +1332,10 @@
         <v>44765</v>
       </c>
       <c r="D13" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G13" t="str">
         <f t="shared" si="0"/>
@@ -1315,13 +1346,19 @@
         <v>1</v>
       </c>
       <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>3</v>
+      </c>
+      <c r="M13">
         <v>0</v>
       </c>
       <c r="N13">
         <v>3</v>
       </c>
       <c r="O13" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="Q13">
         <v>0</v>
@@ -1329,7 +1366,7 @@
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B14" s="3">
         <v>44760</v>
@@ -1338,10 +1375,10 @@
         <v>44765</v>
       </c>
       <c r="D14" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G14" t="str">
         <f t="shared" si="0"/>
@@ -1353,12 +1390,18 @@
       </c>
       <c r="I14">
         <v>1</v>
+      </c>
+      <c r="L14">
+        <v>7</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
       </c>
       <c r="N14">
         <v>3</v>
       </c>
       <c r="O14" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="Q14">
         <v>0</v>
@@ -1366,7 +1409,7 @@
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B15" s="3">
         <v>44771</v>
@@ -1375,10 +1418,10 @@
         <v>44776</v>
       </c>
       <c r="D15" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E15" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G15" t="str">
         <f t="shared" si="0"/>
@@ -1401,10 +1444,10 @@
         <v>2</v>
       </c>
       <c r="O15" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="P15" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="Q15">
         <v>0</v>
@@ -1412,7 +1455,7 @@
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B16" s="3">
         <v>44771</v>
@@ -1421,10 +1464,10 @@
         <v>44776</v>
       </c>
       <c r="D16" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F16" s="9"/>
       <c r="G16" t="str">
@@ -1448,10 +1491,10 @@
         <v>1</v>
       </c>
       <c r="O16" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="P16" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="Q16">
         <v>0</v>
@@ -1459,7 +1502,7 @@
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B17" s="3">
         <v>44798</v>
@@ -1468,10 +1511,10 @@
         <v>44803</v>
       </c>
       <c r="D17" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G17" t="str">
         <f t="shared" si="0"/>
@@ -1497,7 +1540,7 @@
         <v>2</v>
       </c>
       <c r="O17" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="Q17">
         <v>0</v>
@@ -1505,7 +1548,7 @@
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B18" s="3">
         <v>44798</v>
@@ -1514,10 +1557,10 @@
         <v>44803</v>
       </c>
       <c r="D18" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F18" s="9"/>
       <c r="G18" t="str">
@@ -1544,10 +1587,10 @@
         <v>2</v>
       </c>
       <c r="O18" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="P18" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="Q18">
         <v>0</v>
@@ -1555,7 +1598,7 @@
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B19" s="3">
         <v>44798</v>
@@ -1564,10 +1607,10 @@
         <v>44803</v>
       </c>
       <c r="D19" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F19" s="9"/>
       <c r="G19" t="str">
@@ -1585,7 +1628,7 @@
         <v>2</v>
       </c>
       <c r="K19" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L19">
         <v>1</v>
@@ -1597,10 +1640,10 @@
         <v>2</v>
       </c>
       <c r="O19" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="P19" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="Q19">
         <v>0</v>
@@ -1608,7 +1651,7 @@
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B20" s="3">
         <v>44823</v>
@@ -1617,10 +1660,10 @@
         <v>44828</v>
       </c>
       <c r="D20" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E20" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G20" t="str">
         <f t="shared" si="0"/>
@@ -1646,21 +1689,21 @@
         <v>2</v>
       </c>
       <c r="O20" s="12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="P20" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="Q20">
         <v>0</v>
       </c>
       <c r="R20" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B21" s="3">
         <v>44823</v>
@@ -1669,10 +1712,10 @@
         <v>44828</v>
       </c>
       <c r="D21" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E21" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G21" t="str">
         <f t="shared" si="0"/>
@@ -1698,21 +1741,21 @@
         <v>2</v>
       </c>
       <c r="O21" s="12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="P21" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="Q21">
         <v>0</v>
       </c>
       <c r="R21" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B22" s="3">
         <v>44830</v>
@@ -1721,10 +1764,10 @@
         <v>44835</v>
       </c>
       <c r="D22" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E22" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G22" t="str">
         <f t="shared" si="0"/>
@@ -1750,10 +1793,10 @@
         <v>2</v>
       </c>
       <c r="O22" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="P22" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="Q22">
         <v>0</v>
@@ -1761,7 +1804,7 @@
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B23" s="3">
         <v>44830</v>
@@ -1770,10 +1813,10 @@
         <v>44835</v>
       </c>
       <c r="D23" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E23" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G23" t="str">
         <f t="shared" si="0"/>
@@ -1799,10 +1842,10 @@
         <v>2</v>
       </c>
       <c r="O23" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="P23" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="Q23">
         <v>0</v>
@@ -1810,7 +1853,7 @@
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B24" s="3">
         <v>44830</v>
@@ -1819,10 +1862,10 @@
         <v>44835</v>
       </c>
       <c r="D24" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E24" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G24" t="str">
         <f t="shared" si="0"/>
@@ -1848,10 +1891,10 @@
         <v>2</v>
       </c>
       <c r="O24" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="P24" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="Q24">
         <v>0</v>
@@ -1859,7 +1902,7 @@
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B25" s="3">
         <v>44841</v>
@@ -1868,10 +1911,10 @@
         <v>44845</v>
       </c>
       <c r="D25" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F25" s="9"/>
       <c r="G25" t="str">
@@ -1889,7 +1932,7 @@
         <v>3</v>
       </c>
       <c r="K25" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="L25">
         <v>7</v>
@@ -1901,10 +1944,10 @@
         <v>1</v>
       </c>
       <c r="O25" s="9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="P25" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="Q25">
         <v>0</v>
@@ -1912,7 +1955,7 @@
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B26" s="3">
         <v>44841</v>
@@ -1921,10 +1964,10 @@
         <v>44845</v>
       </c>
       <c r="D26" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F26" s="9"/>
       <c r="G26" t="str">
@@ -1942,7 +1985,7 @@
         <v>3</v>
       </c>
       <c r="K26" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="L26">
         <v>9</v>
@@ -1954,10 +1997,10 @@
         <v>1</v>
       </c>
       <c r="O26" s="9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="P26" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="Q26">
         <v>0</v>
@@ -1965,7 +2008,7 @@
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B27" s="3">
         <v>44862</v>
@@ -1974,10 +2017,10 @@
         <v>44867</v>
       </c>
       <c r="D27" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E27" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G27" t="str">
         <f t="shared" si="0"/>
@@ -1994,7 +2037,7 @@
         <v>2</v>
       </c>
       <c r="K27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L27">
         <v>11</v>
@@ -2006,10 +2049,10 @@
         <v>1</v>
       </c>
       <c r="O27" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="P27" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="Q27">
         <v>0</v>
@@ -2017,7 +2060,7 @@
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B28" s="3">
         <v>44862</v>
@@ -2026,10 +2069,10 @@
         <v>44867</v>
       </c>
       <c r="D28" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F28" s="11"/>
       <c r="G28" t="str">
@@ -2047,7 +2090,7 @@
         <v>2</v>
       </c>
       <c r="K28" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L28">
         <v>13</v>
@@ -2059,10 +2102,10 @@
         <v>1</v>
       </c>
       <c r="O28" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="P28" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="Q28">
         <v>0</v>
@@ -2070,7 +2113,7 @@
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B29" s="3">
         <v>44862</v>
@@ -2079,10 +2122,10 @@
         <v>44867</v>
       </c>
       <c r="D29" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F29" s="11"/>
       <c r="G29" t="str">
@@ -2100,7 +2143,7 @@
         <v>2</v>
       </c>
       <c r="K29" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L29">
         <v>11</v>
@@ -2112,10 +2155,10 @@
         <v>1</v>
       </c>
       <c r="O29" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="P29" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="Q29">
         <v>0</v>
@@ -2123,7 +2166,7 @@
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B30" s="3">
         <v>44862</v>
@@ -2132,10 +2175,10 @@
         <v>44867</v>
       </c>
       <c r="D30" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F30" s="11"/>
       <c r="G30" t="str">
@@ -2153,7 +2196,7 @@
         <v>2</v>
       </c>
       <c r="K30" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L30">
         <v>9</v>
@@ -2165,10 +2208,10 @@
         <v>1</v>
       </c>
       <c r="O30" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="P30" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="Q30">
         <v>0</v>
@@ -2176,7 +2219,7 @@
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B31" s="3">
         <v>44911</v>
@@ -2185,10 +2228,10 @@
         <v>44916</v>
       </c>
       <c r="D31" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E31" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G31" t="str">
         <f t="shared" si="0"/>
@@ -2208,10 +2251,10 @@
         <v>2</v>
       </c>
       <c r="O31" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="P31" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="Q31">
         <v>0</v>
@@ -2219,7 +2262,7 @@
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B32" s="3">
         <v>44911</v>
@@ -2228,10 +2271,10 @@
         <v>44916</v>
       </c>
       <c r="D32" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E32" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G32" t="str">
         <f t="shared" si="0"/>
@@ -2251,10 +2294,10 @@
         <v>2</v>
       </c>
       <c r="O32" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="P32" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="Q32">
         <v>0</v>
@@ -2262,7 +2305,7 @@
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B33" s="3">
         <v>44911</v>
@@ -2271,10 +2314,10 @@
         <v>44916</v>
       </c>
       <c r="D33" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E33" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G33" t="str">
         <f t="shared" si="0"/>
@@ -2294,10 +2337,10 @@
         <v>2</v>
       </c>
       <c r="O33" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="P33" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="Q33">
         <v>0</v>
@@ -2305,7 +2348,7 @@
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B34" s="3">
         <v>44932</v>
@@ -2314,10 +2357,10 @@
         <v>44937</v>
       </c>
       <c r="D34" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E34" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G34" t="str">
         <f t="shared" si="0"/>
@@ -2339,7 +2382,7 @@
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B35" s="3">
         <v>44932</v>
@@ -2348,10 +2391,10 @@
         <v>44937</v>
       </c>
       <c r="D35" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E35" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G35" t="str">
         <f t="shared" si="0"/>
@@ -2368,7 +2411,7 @@
         <v>2</v>
       </c>
       <c r="K35" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Q35">
         <v>0</v>
@@ -2376,7 +2419,7 @@
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B36" s="3">
         <v>44932</v>
@@ -2385,10 +2428,10 @@
         <v>44937</v>
       </c>
       <c r="D36" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E36" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G36" t="str">
         <f t="shared" si="0"/>
@@ -2405,7 +2448,7 @@
         <v>2</v>
       </c>
       <c r="K36" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Q36">
         <v>0</v>
@@ -2413,7 +2456,7 @@
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B37" s="3">
         <v>44932</v>
@@ -2422,10 +2465,10 @@
         <v>44937</v>
       </c>
       <c r="D37" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E37" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G37" t="str">
         <f t="shared" si="0"/>
@@ -2447,7 +2490,7 @@
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B38" s="3">
         <v>44932</v>
@@ -2456,13 +2499,13 @@
         <v>44937</v>
       </c>
       <c r="D38" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E38" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F38" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G38" t="str">
         <f t="shared" si="0"/>
@@ -2484,7 +2527,7 @@
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B39" s="3">
         <v>44932</v>
@@ -2493,13 +2536,13 @@
         <v>44937</v>
       </c>
       <c r="D39" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E39" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F39" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G39" t="str">
         <f t="shared" si="0"/>
@@ -2521,7 +2564,7 @@
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B40" s="3">
         <v>44932</v>
@@ -2530,13 +2573,13 @@
         <v>44937</v>
       </c>
       <c r="D40" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E40" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F40" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G40" t="str">
         <f t="shared" si="0"/>
@@ -2553,7 +2596,7 @@
         <v>2</v>
       </c>
       <c r="K40" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Q40">
         <v>0</v>
@@ -2561,7 +2604,7 @@
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B41" s="3">
         <v>44932</v>
@@ -2570,13 +2613,13 @@
         <v>44937</v>
       </c>
       <c r="D41" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E41" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F41" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G41" t="str">
         <f t="shared" si="0"/>
@@ -2593,7 +2636,7 @@
         <v>2</v>
       </c>
       <c r="K41" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Q41">
         <v>0</v>
@@ -2601,7 +2644,7 @@
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B42" s="3">
         <v>44932</v>
@@ -2610,13 +2653,13 @@
         <v>44937</v>
       </c>
       <c r="D42" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E42" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F42" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G42" t="str">
         <f t="shared" si="0"/>
@@ -2633,7 +2676,7 @@
         <v>2</v>
       </c>
       <c r="K42" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Q42">
         <v>0</v>
@@ -2641,7 +2684,7 @@
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B43" s="3">
         <v>44932</v>
@@ -2650,13 +2693,13 @@
         <v>44937</v>
       </c>
       <c r="D43" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E43" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F43" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G43" t="str">
         <f t="shared" si="0"/>
@@ -2673,7 +2716,7 @@
         <v>2</v>
       </c>
       <c r="K43" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Q43">
         <v>0</v>

</xml_diff>

<commit_message>
Fixed some bugs that I ran into while doing an entire run
</commit_message>
<xml_diff>
--- a/resources/Screening_overview.xlsx
+++ b/resources/Screening_overview.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mhuismans/surfdrive/Promotie/12. STRATEGIC/Analyse 2.0/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50E33B50-A09A-EB48-990E-40B04C153411}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15203FE7-6BFB-774F-915C-3972D4A18A87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28080" yWindow="9460" windowWidth="27700" windowHeight="14800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28940" yWindow="7220" windowWidth="27700" windowHeight="14800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="92">
   <si>
     <t>STR_ID</t>
   </si>
@@ -247,9 +260,6 @@
     <t>OPT0424</t>
   </si>
   <si>
-    <t>STR24</t>
-  </si>
-  <si>
     <t>OPT0039</t>
   </si>
   <si>
@@ -287,6 +297,18 @@
   </si>
   <si>
     <t>Passed_QC</t>
+  </si>
+  <si>
+    <t>STR24A</t>
+  </si>
+  <si>
+    <t>STR24B</t>
+  </si>
+  <si>
+    <t>STR27</t>
+  </si>
+  <si>
+    <t>Analyse</t>
   </si>
 </sst>
 </file>
@@ -630,13 +652,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T43"/>
+  <dimension ref="A1:U47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B24" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R33" sqref="R33"/>
+      <selection pane="bottomRight" activeCell="U48" sqref="Q48:U48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -645,7 +667,7 @@
     <col min="4" max="4" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -701,13 +723,16 @@
         <v>17</v>
       </c>
       <c r="S1" t="s">
+        <v>86</v>
+      </c>
+      <c r="T1" t="s">
         <v>87</v>
       </c>
-      <c r="T1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -744,8 +769,11 @@
       <c r="Q2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -779,8 +807,11 @@
       <c r="Q3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -814,8 +845,11 @@
       <c r="Q4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -852,8 +886,11 @@
       <c r="Q5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -887,8 +924,11 @@
       <c r="Q6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -925,8 +965,11 @@
       <c r="Q7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -972,8 +1015,11 @@
       <c r="T8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -1016,8 +1062,11 @@
       <c r="T9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -1060,8 +1109,11 @@
       <c r="T10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -1104,8 +1156,11 @@
       <c r="T11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -1148,8 +1203,11 @@
       <c r="T12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -1192,8 +1250,11 @@
       <c r="T13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -1236,8 +1297,11 @@
       <c r="T14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -1283,8 +1347,11 @@
       <c r="T15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -1333,8 +1400,11 @@
       <c r="T16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -1380,8 +1450,11 @@
       <c r="T17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>43</v>
       </c>
@@ -1430,8 +1503,11 @@
       <c r="T18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -1483,8 +1559,11 @@
       <c r="T19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>49</v>
       </c>
@@ -1536,8 +1615,11 @@
       <c r="T20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>49</v>
       </c>
@@ -1589,8 +1671,11 @@
       <c r="T21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>54</v>
       </c>
@@ -1639,8 +1724,11 @@
       <c r="T22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>54</v>
       </c>
@@ -1689,8 +1777,11 @@
       <c r="T23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>54</v>
       </c>
@@ -1739,8 +1830,11 @@
       <c r="T24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>59</v>
       </c>
@@ -1792,8 +1886,11 @@
       <c r="T25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>59</v>
       </c>
@@ -1845,8 +1942,11 @@
       <c r="T26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>64</v>
       </c>
@@ -1898,8 +1998,11 @@
       <c r="T27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>64</v>
       </c>
@@ -1951,8 +2054,11 @@
       <c r="T28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>64</v>
       </c>
@@ -2004,8 +2110,11 @@
       <c r="T29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>64</v>
       </c>
@@ -2057,8 +2166,11 @@
       <c r="T30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>70</v>
       </c>
@@ -2104,8 +2216,14 @@
       <c r="Q31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T31">
+        <v>0</v>
+      </c>
+      <c r="U31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>70</v>
       </c>
@@ -2151,8 +2269,14 @@
       <c r="Q32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T32">
+        <v>0</v>
+      </c>
+      <c r="U32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>70</v>
       </c>
@@ -2198,10 +2322,16 @@
       <c r="Q33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T33">
+        <v>0</v>
+      </c>
+      <c r="U33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="B34" s="1">
         <v>44932</v>
@@ -2213,10 +2343,10 @@
         <v>31</v>
       </c>
       <c r="E34" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G34" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H34">
         <v>0</v>
@@ -2230,10 +2360,16 @@
       <c r="Q34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T34">
+        <v>0</v>
+      </c>
+      <c r="U34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="B35" s="1">
         <v>44932</v>
@@ -2260,15 +2396,21 @@
         <v>2</v>
       </c>
       <c r="K35" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="Q35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T35">
+        <v>0</v>
+      </c>
+      <c r="U35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="B36" s="1">
         <v>44932</v>
@@ -2295,15 +2437,21 @@
         <v>2</v>
       </c>
       <c r="K36" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="Q36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T36">
+        <v>0</v>
+      </c>
+      <c r="U36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="B37" s="1">
         <v>44932</v>
@@ -2312,7 +2460,7 @@
         <v>44937</v>
       </c>
       <c r="D37" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E37" t="s">
         <v>73</v>
@@ -2332,10 +2480,16 @@
       <c r="Q37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T37">
+        <v>0</v>
+      </c>
+      <c r="U37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="B38" s="1">
         <v>44932</v>
@@ -2344,17 +2498,17 @@
         <v>44937</v>
       </c>
       <c r="D38" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E38" t="s">
         <v>73</v>
       </c>
       <c r="F38" t="s">
+        <v>78</v>
+      </c>
+      <c r="G38" t="s">
         <v>79</v>
       </c>
-      <c r="G38" t="s">
-        <v>80</v>
-      </c>
       <c r="H38">
         <v>0</v>
       </c>
@@ -2367,10 +2521,16 @@
       <c r="Q38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T38">
+        <v>0</v>
+      </c>
+      <c r="U38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="B39" s="1">
         <v>44932</v>
@@ -2379,17 +2539,17 @@
         <v>44937</v>
       </c>
       <c r="D39" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E39" t="s">
         <v>73</v>
       </c>
       <c r="F39" t="s">
+        <v>80</v>
+      </c>
+      <c r="G39" t="s">
         <v>81</v>
       </c>
-      <c r="G39" t="s">
-        <v>82</v>
-      </c>
       <c r="H39">
         <v>0</v>
       </c>
@@ -2402,10 +2562,16 @@
       <c r="Q39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T39">
+        <v>0</v>
+      </c>
+      <c r="U39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="B40" s="1">
         <v>44932</v>
@@ -2414,16 +2580,16 @@
         <v>44937</v>
       </c>
       <c r="D40" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E40" t="s">
         <v>71</v>
       </c>
       <c r="F40" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G40" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H40">
         <v>0</v>
@@ -2435,15 +2601,21 @@
         <v>2</v>
       </c>
       <c r="K40" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="Q40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T40">
+        <v>0</v>
+      </c>
+      <c r="U40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="B41" s="1">
         <v>44932</v>
@@ -2452,16 +2624,16 @@
         <v>44937</v>
       </c>
       <c r="D41" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E41" t="s">
         <v>71</v>
       </c>
       <c r="F41" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G41" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H41">
         <v>0</v>
@@ -2473,15 +2645,21 @@
         <v>2</v>
       </c>
       <c r="K41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="Q41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T41">
+        <v>0</v>
+      </c>
+      <c r="U41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="B42" s="1">
         <v>44932</v>
@@ -2490,16 +2668,16 @@
         <v>44937</v>
       </c>
       <c r="D42" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E42" t="s">
         <v>74</v>
       </c>
       <c r="F42" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G42" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H42">
         <v>0</v>
@@ -2511,15 +2689,21 @@
         <v>2</v>
       </c>
       <c r="K42" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="Q42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T42">
+        <v>0</v>
+      </c>
+      <c r="U42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="B43" s="1">
         <v>44932</v>
@@ -2528,16 +2712,16 @@
         <v>44937</v>
       </c>
       <c r="D43" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E43" t="s">
         <v>74</v>
       </c>
       <c r="F43" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G43" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H43">
         <v>0</v>
@@ -2549,10 +2733,216 @@
         <v>2</v>
       </c>
       <c r="K43" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="Q43">
         <v>0</v>
+      </c>
+      <c r="T43">
+        <v>0</v>
+      </c>
+      <c r="U43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>90</v>
+      </c>
+      <c r="B44" s="1">
+        <v>44939</v>
+      </c>
+      <c r="C44" s="1">
+        <v>44944</v>
+      </c>
+      <c r="D44" t="s">
+        <v>31</v>
+      </c>
+      <c r="E44" t="s">
+        <v>60</v>
+      </c>
+      <c r="G44" t="s">
+        <v>60</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+      <c r="I44">
+        <v>1</v>
+      </c>
+      <c r="J44">
+        <v>3</v>
+      </c>
+      <c r="L44">
+        <v>3</v>
+      </c>
+      <c r="M44">
+        <v>0</v>
+      </c>
+      <c r="N44">
+        <v>3</v>
+      </c>
+      <c r="O44" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q44">
+        <v>0</v>
+      </c>
+      <c r="T44">
+        <v>0</v>
+      </c>
+      <c r="U44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>90</v>
+      </c>
+      <c r="B45" s="1">
+        <v>44939</v>
+      </c>
+      <c r="C45" s="1">
+        <v>44944</v>
+      </c>
+      <c r="D45" t="s">
+        <v>31</v>
+      </c>
+      <c r="E45" t="s">
+        <v>47</v>
+      </c>
+      <c r="G45" t="s">
+        <v>47</v>
+      </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
+      <c r="I45">
+        <v>1</v>
+      </c>
+      <c r="J45">
+        <v>3</v>
+      </c>
+      <c r="L45">
+        <v>1</v>
+      </c>
+      <c r="M45">
+        <v>0</v>
+      </c>
+      <c r="N45">
+        <v>3</v>
+      </c>
+      <c r="O45" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q45">
+        <v>0</v>
+      </c>
+      <c r="T45">
+        <v>0</v>
+      </c>
+      <c r="U45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>90</v>
+      </c>
+      <c r="B46" s="1">
+        <v>44939</v>
+      </c>
+      <c r="C46" s="1">
+        <v>44944</v>
+      </c>
+      <c r="D46" t="s">
+        <v>31</v>
+      </c>
+      <c r="E46" t="s">
+        <v>63</v>
+      </c>
+      <c r="G46" t="s">
+        <v>63</v>
+      </c>
+      <c r="H46">
+        <v>1</v>
+      </c>
+      <c r="I46">
+        <v>0</v>
+      </c>
+      <c r="J46">
+        <v>3</v>
+      </c>
+      <c r="L46">
+        <v>7</v>
+      </c>
+      <c r="M46">
+        <v>0</v>
+      </c>
+      <c r="N46">
+        <v>3</v>
+      </c>
+      <c r="O46" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q46">
+        <v>0</v>
+      </c>
+      <c r="T46">
+        <v>0</v>
+      </c>
+      <c r="U46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>90</v>
+      </c>
+      <c r="B47" s="1">
+        <v>44939</v>
+      </c>
+      <c r="C47" s="1">
+        <v>44944</v>
+      </c>
+      <c r="D47" t="s">
+        <v>31</v>
+      </c>
+      <c r="E47" t="s">
+        <v>45</v>
+      </c>
+      <c r="G47" t="s">
+        <v>45</v>
+      </c>
+      <c r="H47">
+        <v>1</v>
+      </c>
+      <c r="I47">
+        <v>0</v>
+      </c>
+      <c r="J47">
+        <v>3</v>
+      </c>
+      <c r="L47">
+        <v>5</v>
+      </c>
+      <c r="M47">
+        <v>0</v>
+      </c>
+      <c r="N47">
+        <v>3</v>
+      </c>
+      <c r="O47" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q47">
+        <v>0</v>
+      </c>
+      <c r="T47">
+        <v>0</v>
+      </c>
+      <c r="U47">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added QC plots that can facilitate easy identification of good and bad experimetns
</commit_message>
<xml_diff>
--- a/resources/Screening_overview.xlsx
+++ b/resources/Screening_overview.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mhuismans/surfdrive/Promotie/12. STRATEGIC/Analyse 2.0/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15203FE7-6BFB-774F-915C-3972D4A18A87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{391FB2DF-98B3-874F-B214-18CEF08BFB99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28940" yWindow="7220" windowWidth="27700" windowHeight="14800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="660" yWindow="860" windowWidth="27700" windowHeight="14800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet 1'!$A$1:$W$50</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="95">
   <si>
     <t>STR_ID</t>
   </si>
@@ -272,27 +275,9 @@
     <t>WNT_high</t>
   </si>
   <si>
-    <t>OPT0030_WNT_high</t>
-  </si>
-  <si>
     <t>WNT_low</t>
   </si>
   <si>
-    <t>OPT0030_WNT_low</t>
-  </si>
-  <si>
-    <t>OPT0024_WNT_high</t>
-  </si>
-  <si>
-    <t>OPT0024_WNT_low</t>
-  </si>
-  <si>
-    <t>OPT0424_WNT_high</t>
-  </si>
-  <si>
-    <t>OPT0424_WNT_low</t>
-  </si>
-  <si>
     <t>Curve_comments</t>
   </si>
   <si>
@@ -309,6 +294,33 @@
   </si>
   <si>
     <t>Analyse</t>
+  </si>
+  <si>
+    <t>STR26</t>
+  </si>
+  <si>
+    <t>FullscreenV3.xlsx</t>
+  </si>
+  <si>
+    <t>OPT0421</t>
+  </si>
+  <si>
+    <t>RAS28</t>
+  </si>
+  <si>
+    <t>Niet goed de CTG toegevoegd</t>
+  </si>
+  <si>
+    <t>Demi</t>
+  </si>
+  <si>
+    <t>FullscreenV2_inverted.xlsx</t>
+  </si>
+  <si>
+    <t>Tween_bad</t>
+  </si>
+  <si>
+    <t>DMSO_bad</t>
   </si>
 </sst>
 </file>
@@ -652,42 +664,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U47"/>
+  <dimension ref="A1:W50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D25" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="S29" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="U48" sqref="Q48:U48"/>
+      <selection pane="bottomRight" activeCell="V51" sqref="V51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" customWidth="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H1" t="s">
         <v>7</v>
@@ -723,39 +736,46 @@
         <v>17</v>
       </c>
       <c r="S1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="T1" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="U1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+      <c r="V1" t="s">
+        <v>93</v>
+      </c>
+      <c r="W1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="str">
+        <f>IF(NOT(ISBLANK(C2)),B2&amp;"_"&amp;C2,B2)</f>
+        <v>OPT0016</v>
+      </c>
+      <c r="E2" s="1">
         <v>44670</v>
       </c>
-      <c r="C2" s="1">
+      <c r="F2" s="1">
         <v>44675</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
         <v>19</v>
       </c>
-      <c r="E2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" t="s">
-        <v>20</v>
-      </c>
       <c r="H2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N2">
         <v>0</v>
@@ -763,34 +783,35 @@
       <c r="O2" t="s">
         <v>21</v>
       </c>
-      <c r="P2" t="s">
-        <v>22</v>
-      </c>
       <c r="Q2">
         <v>0</v>
       </c>
       <c r="U2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" t="str">
+        <f>IF(NOT(ISBLANK(C3)),B3&amp;"_"&amp;C3,B3)</f>
+        <v>OPT0112</v>
+      </c>
+      <c r="E3" s="1">
         <v>44670</v>
       </c>
-      <c r="C3" s="1">
+      <c r="F3" s="1">
         <v>44675</v>
       </c>
-      <c r="D3" t="s">
+      <c r="G3" t="s">
         <v>19</v>
-      </c>
-      <c r="E3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" t="s">
-        <v>23</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -810,31 +831,35 @@
       <c r="U3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="str">
+        <f>IF(NOT(ISBLANK(C4)),B4&amp;"_"&amp;C4,B4)</f>
+        <v>RAS04</v>
+      </c>
+      <c r="E4" s="1">
         <v>44670</v>
       </c>
-      <c r="C4" s="1">
+      <c r="F4" s="1">
         <v>44675</v>
       </c>
-      <c r="D4" t="s">
+      <c r="G4" t="s">
         <v>19</v>
       </c>
-      <c r="E4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" t="s">
-        <v>24</v>
-      </c>
       <c r="H4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N4">
         <v>0</v>
@@ -842,37 +867,44 @@
       <c r="O4" t="s">
         <v>21</v>
       </c>
+      <c r="P4" t="s">
+        <v>22</v>
+      </c>
       <c r="Q4">
         <v>0</v>
       </c>
       <c r="U4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" t="str">
+        <f>IF(NOT(ISBLANK(C5)),B5&amp;"_"&amp;C5,B5)</f>
+        <v>OPT0014</v>
+      </c>
+      <c r="E5" s="1">
         <v>44679</v>
       </c>
-      <c r="C5" s="1">
+      <c r="F5" s="1">
         <v>44683</v>
       </c>
-      <c r="D5" t="s">
+      <c r="G5" t="s">
         <v>19</v>
       </c>
-      <c r="E5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" t="s">
-        <v>26</v>
-      </c>
       <c r="H5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N5">
         <v>0</v>
@@ -880,40 +912,41 @@
       <c r="O5" t="s">
         <v>21</v>
       </c>
-      <c r="P5" t="s">
-        <v>22</v>
-      </c>
       <c r="Q5">
         <v>0</v>
       </c>
       <c r="U5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" t="str">
+        <f>IF(NOT(ISBLANK(C6)),B6&amp;"_"&amp;C6,B6)</f>
+        <v>RAS25</v>
+      </c>
+      <c r="E6" s="1">
         <v>44679</v>
       </c>
-      <c r="C6" s="1">
+      <c r="F6" s="1">
         <v>44683</v>
       </c>
-      <c r="D6" t="s">
+      <c r="G6" t="s">
         <v>19</v>
       </c>
-      <c r="E6" t="s">
-        <v>27</v>
-      </c>
-      <c r="G6" t="s">
-        <v>27</v>
-      </c>
       <c r="H6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N6">
         <v>0</v>
@@ -921,31 +954,38 @@
       <c r="O6" t="s">
         <v>21</v>
       </c>
+      <c r="P6" t="s">
+        <v>22</v>
+      </c>
       <c r="Q6">
         <v>0</v>
       </c>
       <c r="U6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" t="str">
+        <f>IF(NOT(ISBLANK(C7)),B7&amp;"_"&amp;C7,B7)</f>
+        <v>RAS21</v>
+      </c>
+      <c r="E7" s="1">
         <v>44706</v>
       </c>
-      <c r="C7" s="1">
+      <c r="F7" s="1">
         <v>44711</v>
       </c>
-      <c r="D7" t="s">
+      <c r="G7" t="s">
         <v>19</v>
-      </c>
-      <c r="E7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G7" t="s">
-        <v>29</v>
       </c>
       <c r="H7">
         <v>1</v>
@@ -968,25 +1008,29 @@
       <c r="U7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" t="str">
+        <f>IF(NOT(ISBLANK(C8)),B8&amp;"_"&amp;C8,B8)</f>
+        <v>OPT0015</v>
+      </c>
+      <c r="E8" s="1">
         <v>44741</v>
       </c>
-      <c r="C8" s="1">
+      <c r="F8" s="1">
         <v>44746</v>
       </c>
-      <c r="D8" t="s">
+      <c r="G8" t="s">
         <v>31</v>
-      </c>
-      <c r="E8" t="s">
-        <v>32</v>
-      </c>
-      <c r="G8" t="s">
-        <v>32</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -1018,25 +1062,32 @@
       <c r="U8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" t="str">
+        <f>IF(NOT(ISBLANK(C9)),B9&amp;"_"&amp;C9,B9)</f>
+        <v>RAS04</v>
+      </c>
+      <c r="E9" s="1">
         <v>44741</v>
       </c>
-      <c r="C9" s="1">
+      <c r="F9" s="1">
         <v>44746</v>
       </c>
-      <c r="D9" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" t="s">
-        <v>20</v>
-      </c>
       <c r="G9" t="s">
-        <v>20</v>
+        <v>92</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -1057,7 +1108,7 @@
         <v>21</v>
       </c>
       <c r="Q9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T9">
         <v>0</v>
@@ -1065,25 +1116,32 @@
       <c r="U9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V9">
+        <v>1</v>
+      </c>
+      <c r="W9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" t="str">
+        <f>IF(NOT(ISBLANK(C10)),B10&amp;"_"&amp;C10,B10)</f>
+        <v>OPT0016</v>
+      </c>
+      <c r="E10" s="1">
         <v>44750</v>
       </c>
-      <c r="C10" s="1">
+      <c r="F10" s="1">
         <v>44755</v>
       </c>
-      <c r="D10" t="s">
+      <c r="G10" t="s">
         <v>31</v>
-      </c>
-      <c r="E10" t="s">
-        <v>24</v>
-      </c>
-      <c r="G10" t="s">
-        <v>24</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -1112,34 +1170,41 @@
       <c r="U10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V10">
+        <v>0</v>
+      </c>
+      <c r="W10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" t="str">
+        <f>IF(NOT(ISBLANK(C11)),B11&amp;"_"&amp;C11,B11)</f>
+        <v>OPT0112</v>
+      </c>
+      <c r="E11" s="1">
         <v>44750</v>
       </c>
-      <c r="C11" s="1">
+      <c r="F11" s="1">
         <v>44755</v>
       </c>
-      <c r="D11" t="s">
+      <c r="G11" t="s">
         <v>31</v>
       </c>
-      <c r="E11" t="s">
-        <v>26</v>
-      </c>
-      <c r="G11" t="s">
-        <v>26</v>
-      </c>
       <c r="H11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L11">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="M11">
         <v>0</v>
@@ -1154,39 +1219,46 @@
         <v>0</v>
       </c>
       <c r="T11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V11">
+        <v>1</v>
+      </c>
+      <c r="W11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" t="str">
+        <f>IF(NOT(ISBLANK(C12)),B12&amp;"_"&amp;C12,B12)</f>
+        <v>RAS25</v>
+      </c>
+      <c r="E12" s="1">
         <v>44750</v>
       </c>
-      <c r="C12" s="1">
+      <c r="F12" s="1">
         <v>44755</v>
       </c>
-      <c r="D12" t="s">
+      <c r="G12" t="s">
         <v>31</v>
       </c>
-      <c r="E12" t="s">
-        <v>23</v>
-      </c>
-      <c r="G12" t="s">
-        <v>23</v>
-      </c>
       <c r="H12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="M12">
         <v>0</v>
@@ -1206,34 +1278,41 @@
       <c r="U12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V12">
+        <v>0</v>
+      </c>
+      <c r="W12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" t="str">
+        <f>IF(NOT(ISBLANK(C13)),B13&amp;"_"&amp;C13,B13)</f>
+        <v>OPT0014</v>
+      </c>
+      <c r="E13" s="1">
         <v>44760</v>
       </c>
-      <c r="C13" s="1">
+      <c r="F13" s="1">
         <v>44765</v>
       </c>
-      <c r="D13" t="s">
+      <c r="G13" t="s">
         <v>31</v>
       </c>
-      <c r="E13" t="s">
-        <v>29</v>
-      </c>
-      <c r="G13" t="s">
-        <v>29</v>
-      </c>
       <c r="H13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L13">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="M13">
         <v>0</v>
@@ -1253,34 +1332,41 @@
       <c r="U13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V13">
+        <v>0</v>
+      </c>
+      <c r="W13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" t="str">
+        <f>IF(NOT(ISBLANK(C14)),B14&amp;"_"&amp;C14,B14)</f>
+        <v>RAS21</v>
+      </c>
+      <c r="E14" s="1">
         <v>44760</v>
       </c>
-      <c r="C14" s="1">
+      <c r="F14" s="1">
         <v>44765</v>
       </c>
-      <c r="D14" t="s">
+      <c r="G14" t="s">
         <v>31</v>
       </c>
-      <c r="E14" t="s">
-        <v>27</v>
-      </c>
-      <c r="G14" t="s">
-        <v>27</v>
-      </c>
       <c r="H14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L14">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="M14">
         <v>0</v>
@@ -1300,26 +1386,33 @@
       <c r="U14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V14">
+        <v>0</v>
+      </c>
+      <c r="W14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" t="str">
+        <f>IF(NOT(ISBLANK(C15)),B15&amp;"_"&amp;C15,B15)</f>
+        <v>HUB-02-C2-89</v>
+      </c>
+      <c r="E15" s="1">
         <v>44771</v>
       </c>
-      <c r="C15" s="1">
+      <c r="F15" s="1">
         <v>44776</v>
       </c>
-      <c r="D15" t="s">
+      <c r="G15" t="s">
         <v>31</v>
       </c>
-      <c r="E15" t="s">
-        <v>37</v>
-      </c>
-      <c r="G15" t="s">
-        <v>37</v>
-      </c>
       <c r="H15">
         <v>0</v>
       </c>
@@ -1327,49 +1420,59 @@
         <v>1</v>
       </c>
       <c r="L15">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="M15">
         <v>1</v>
       </c>
       <c r="N15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O15" t="s">
         <v>38</v>
       </c>
       <c r="P15" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="Q15">
         <v>0</v>
       </c>
+      <c r="R15" t="s">
+        <v>42</v>
+      </c>
       <c r="T15">
         <v>1</v>
       </c>
       <c r="U15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V15">
+        <v>0</v>
+      </c>
+      <c r="W15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" t="str">
+        <f>IF(NOT(ISBLANK(C16)),B16&amp;"_"&amp;C16,B16)</f>
+        <v>OPT0005</v>
+      </c>
+      <c r="E16" s="1">
         <v>44771</v>
       </c>
-      <c r="C16" s="1">
+      <c r="F16" s="1">
         <v>44776</v>
       </c>
-      <c r="D16" t="s">
+      <c r="G16" t="s">
         <v>31</v>
       </c>
-      <c r="E16" t="s">
-        <v>40</v>
-      </c>
-      <c r="G16" t="s">
-        <v>40</v>
-      </c>
       <c r="H16">
         <v>0</v>
       </c>
@@ -1377,66 +1480,73 @@
         <v>1</v>
       </c>
       <c r="L16">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="M16">
         <v>1</v>
       </c>
       <c r="N16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O16" t="s">
         <v>38</v>
       </c>
       <c r="P16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="Q16">
         <v>0</v>
       </c>
-      <c r="R16" t="s">
-        <v>42</v>
-      </c>
       <c r="T16">
         <v>1</v>
       </c>
       <c r="U16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V16">
+        <v>0</v>
+      </c>
+      <c r="W16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" t="str">
+        <f>IF(NOT(ISBLANK(C17)),B17&amp;"_"&amp;C17,B17)</f>
+        <v>OPT0413</v>
+      </c>
+      <c r="E17" s="1">
         <v>44798</v>
       </c>
-      <c r="C17" s="1">
+      <c r="F17" s="1">
         <v>44803</v>
       </c>
-      <c r="D17" t="s">
+      <c r="G17" t="s">
         <v>31</v>
       </c>
-      <c r="E17" t="s">
-        <v>44</v>
-      </c>
-      <c r="G17" t="s">
-        <v>44</v>
-      </c>
       <c r="H17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J17">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="K17" t="s">
+        <v>48</v>
       </c>
       <c r="L17">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="M17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N17">
         <v>2</v>
@@ -1444,6 +1554,9 @@
       <c r="O17" t="s">
         <v>21</v>
       </c>
+      <c r="P17" t="s">
+        <v>46</v>
+      </c>
       <c r="Q17">
         <v>0</v>
       </c>
@@ -1453,26 +1566,33 @@
       <c r="U17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V17">
+        <v>0</v>
+      </c>
+      <c r="W17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>43</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" t="str">
+        <f>IF(NOT(ISBLANK(C18)),B18&amp;"_"&amp;C18,B18)</f>
+        <v>RAS12</v>
+      </c>
+      <c r="E18" s="1">
         <v>44798</v>
       </c>
-      <c r="C18" s="1">
+      <c r="F18" s="1">
         <v>44803</v>
       </c>
-      <c r="D18" t="s">
+      <c r="G18" t="s">
         <v>31</v>
       </c>
-      <c r="E18" t="s">
-        <v>45</v>
-      </c>
-      <c r="G18" t="s">
-        <v>45</v>
-      </c>
       <c r="H18">
         <v>1</v>
       </c>
@@ -1483,7 +1603,7 @@
         <v>3</v>
       </c>
       <c r="L18">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="M18">
         <v>1</v>
@@ -1494,9 +1614,6 @@
       <c r="O18" t="s">
         <v>21</v>
       </c>
-      <c r="P18" t="s">
-        <v>46</v>
-      </c>
       <c r="Q18">
         <v>0</v>
       </c>
@@ -1506,43 +1623,47 @@
       <c r="U18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V18">
+        <v>0</v>
+      </c>
+      <c r="W18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>43</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" t="str">
+        <f>IF(NOT(ISBLANK(C19)),B19&amp;"_"&amp;C19,B19)</f>
+        <v>RAS27</v>
+      </c>
+      <c r="E19" s="1">
         <v>44798</v>
       </c>
-      <c r="C19" s="1">
+      <c r="F19" s="1">
         <v>44803</v>
       </c>
-      <c r="D19" t="s">
+      <c r="G19" t="s">
         <v>31</v>
       </c>
-      <c r="E19" t="s">
-        <v>47</v>
-      </c>
-      <c r="G19" t="s">
-        <v>47</v>
-      </c>
       <c r="H19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J19">
-        <v>2</v>
-      </c>
-      <c r="K19" t="s">
-        <v>48</v>
+        <v>3</v>
       </c>
       <c r="L19">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="M19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N19">
         <v>2</v>
@@ -1562,40 +1683,47 @@
       <c r="U19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V19">
+        <v>0</v>
+      </c>
+      <c r="W19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" t="str">
+        <f>IF(NOT(ISBLANK(C20)),B20&amp;"_"&amp;C20,B20)</f>
+        <v>OPT0419</v>
+      </c>
+      <c r="E20" s="1">
         <v>44823</v>
       </c>
-      <c r="C20" s="1">
+      <c r="F20" s="1">
         <v>44828</v>
       </c>
-      <c r="D20" t="s">
+      <c r="G20" t="s">
         <v>31</v>
       </c>
-      <c r="E20" t="s">
-        <v>50</v>
-      </c>
-      <c r="G20" t="s">
-        <v>50</v>
-      </c>
       <c r="H20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J20">
         <v>2</v>
       </c>
       <c r="L20">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="M20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N20">
         <v>2</v>
@@ -1618,40 +1746,47 @@
       <c r="U20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V20">
+        <v>1</v>
+      </c>
+      <c r="W20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>49</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" t="str">
+        <f>IF(NOT(ISBLANK(C21)),B21&amp;"_"&amp;C21,B21)</f>
+        <v>RAS05</v>
+      </c>
+      <c r="E21" s="1">
         <v>44823</v>
       </c>
-      <c r="C21" s="1">
+      <c r="F21" s="1">
         <v>44828</v>
       </c>
-      <c r="D21" t="s">
+      <c r="G21" t="s">
         <v>31</v>
       </c>
-      <c r="E21" t="s">
-        <v>53</v>
-      </c>
-      <c r="G21" t="s">
-        <v>53</v>
-      </c>
       <c r="H21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J21">
         <v>2</v>
       </c>
       <c r="L21">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="M21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N21">
         <v>2</v>
@@ -1674,37 +1809,44 @@
       <c r="U21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V21">
+        <v>1</v>
+      </c>
+      <c r="W21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>54</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" t="s">
+        <v>58</v>
+      </c>
+      <c r="D22" t="str">
+        <f>IF(NOT(ISBLANK(C22)),B22&amp;"_"&amp;C22,B22)</f>
+        <v>OPT0408</v>
+      </c>
+      <c r="E22" s="1">
         <v>44830</v>
       </c>
-      <c r="C22" s="1">
+      <c r="F22" s="1">
         <v>44835</v>
       </c>
-      <c r="D22" t="s">
+      <c r="G22" t="s">
         <v>31</v>
       </c>
-      <c r="E22" t="s">
-        <v>55</v>
-      </c>
-      <c r="G22" t="s">
-        <v>55</v>
-      </c>
       <c r="H22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J22">
         <v>3</v>
       </c>
       <c r="L22">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="M22">
         <v>0</v>
@@ -1727,26 +1869,33 @@
       <c r="U22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V22">
+        <v>0</v>
+      </c>
+      <c r="W22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>54</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23" t="s">
+        <v>55</v>
+      </c>
+      <c r="D23" t="str">
+        <f>IF(NOT(ISBLANK(C23)),B23&amp;"_"&amp;C23,B23)</f>
+        <v>RAS06</v>
+      </c>
+      <c r="E23" s="1">
         <v>44830</v>
       </c>
-      <c r="C23" s="1">
+      <c r="F23" s="1">
         <v>44835</v>
       </c>
-      <c r="D23" t="s">
+      <c r="G23" t="s">
         <v>31</v>
       </c>
-      <c r="E23" t="s">
-        <v>57</v>
-      </c>
-      <c r="G23" t="s">
-        <v>57</v>
-      </c>
       <c r="H23">
         <v>1</v>
       </c>
@@ -1757,7 +1906,7 @@
         <v>3</v>
       </c>
       <c r="L23">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M23">
         <v>0</v>
@@ -1780,37 +1929,44 @@
       <c r="U23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V23">
+        <v>0</v>
+      </c>
+      <c r="W23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>54</v>
       </c>
-      <c r="B24" s="1">
+      <c r="B24" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24" t="str">
+        <f>IF(NOT(ISBLANK(C24)),B24&amp;"_"&amp;C24,B24)</f>
+        <v>RAS13</v>
+      </c>
+      <c r="E24" s="1">
         <v>44830</v>
       </c>
-      <c r="C24" s="1">
+      <c r="F24" s="1">
         <v>44835</v>
       </c>
-      <c r="D24" t="s">
+      <c r="G24" t="s">
         <v>31</v>
       </c>
-      <c r="E24" t="s">
-        <v>58</v>
-      </c>
-      <c r="G24" t="s">
-        <v>58</v>
-      </c>
       <c r="H24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J24">
         <v>3</v>
       </c>
       <c r="L24">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M24">
         <v>0</v>
@@ -1833,25 +1989,32 @@
       <c r="U24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V24">
+        <v>0</v>
+      </c>
+      <c r="W24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>59</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" t="s">
+        <v>60</v>
+      </c>
+      <c r="D25" t="str">
+        <f>IF(NOT(ISBLANK(C25)),B25&amp;"_"&amp;C25,B25)</f>
+        <v>OPT0034</v>
+      </c>
+      <c r="E25" s="1">
         <v>44841</v>
       </c>
-      <c r="C25" s="1">
+      <c r="F25" s="1">
         <v>44845</v>
       </c>
-      <c r="D25" t="s">
+      <c r="G25" t="s">
         <v>31</v>
-      </c>
-      <c r="E25" t="s">
-        <v>60</v>
-      </c>
-      <c r="G25" t="s">
-        <v>60</v>
       </c>
       <c r="H25">
         <v>0</v>
@@ -1889,25 +2052,32 @@
       <c r="U25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V25">
+        <v>1</v>
+      </c>
+      <c r="W25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>59</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B26" t="s">
+        <v>63</v>
+      </c>
+      <c r="D26" t="str">
+        <f>IF(NOT(ISBLANK(C26)),B26&amp;"_"&amp;C26,B26)</f>
+        <v>RAS11</v>
+      </c>
+      <c r="E26" s="1">
         <v>44841</v>
       </c>
-      <c r="C26" s="1">
+      <c r="F26" s="1">
         <v>44845</v>
       </c>
-      <c r="D26" t="s">
+      <c r="G26" t="s">
         <v>31</v>
-      </c>
-      <c r="E26" t="s">
-        <v>63</v>
-      </c>
-      <c r="G26" t="s">
-        <v>63</v>
       </c>
       <c r="H26">
         <v>1</v>
@@ -1922,10 +2092,10 @@
         <v>61</v>
       </c>
       <c r="L26">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="M26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N26">
         <v>1</v>
@@ -1945,25 +2115,32 @@
       <c r="U26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V26">
+        <v>1</v>
+      </c>
+      <c r="W26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>64</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B27" t="s">
+        <v>65</v>
+      </c>
+      <c r="D27" t="str">
+        <f>IF(NOT(ISBLANK(C27)),B27&amp;"_"&amp;C27,B27)</f>
+        <v>OPT0402</v>
+      </c>
+      <c r="E27" s="1">
         <v>44862</v>
       </c>
-      <c r="C27" s="1">
+      <c r="F27" s="1">
         <v>44867</v>
       </c>
-      <c r="D27" t="s">
+      <c r="G27" t="s">
         <v>31</v>
-      </c>
-      <c r="E27" t="s">
-        <v>65</v>
-      </c>
-      <c r="G27" t="s">
-        <v>65</v>
       </c>
       <c r="H27">
         <v>0</v>
@@ -2001,25 +2178,32 @@
       <c r="U27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V27">
+        <v>1</v>
+      </c>
+      <c r="W27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>64</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28" t="s">
+        <v>67</v>
+      </c>
+      <c r="D28" t="str">
+        <f>IF(NOT(ISBLANK(C28)),B28&amp;"_"&amp;C28,B28)</f>
+        <v>RAS16</v>
+      </c>
+      <c r="E28" s="1">
         <v>44862</v>
       </c>
-      <c r="C28" s="1">
+      <c r="F28" s="1">
         <v>44867</v>
       </c>
-      <c r="D28" t="s">
+      <c r="G28" t="s">
         <v>31</v>
-      </c>
-      <c r="E28" t="s">
-        <v>67</v>
-      </c>
-      <c r="G28" t="s">
-        <v>67</v>
       </c>
       <c r="H28">
         <v>1</v>
@@ -2057,25 +2241,32 @@
       <c r="U28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V28">
+        <v>1</v>
+      </c>
+      <c r="W28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>64</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B29" t="s">
+        <v>68</v>
+      </c>
+      <c r="D29" t="str">
+        <f>IF(NOT(ISBLANK(C29)),B29&amp;"_"&amp;C29,B29)</f>
+        <v>RAS22</v>
+      </c>
+      <c r="E29" s="1">
         <v>44862</v>
       </c>
-      <c r="C29" s="1">
+      <c r="F29" s="1">
         <v>44867</v>
       </c>
-      <c r="D29" t="s">
+      <c r="G29" t="s">
         <v>31</v>
-      </c>
-      <c r="E29" t="s">
-        <v>68</v>
-      </c>
-      <c r="G29" t="s">
-        <v>68</v>
       </c>
       <c r="H29">
         <v>1</v>
@@ -2113,25 +2304,32 @@
       <c r="U29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V29">
+        <v>1</v>
+      </c>
+      <c r="W29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>64</v>
       </c>
-      <c r="B30" s="1">
+      <c r="B30" t="s">
+        <v>69</v>
+      </c>
+      <c r="D30" t="str">
+        <f>IF(NOT(ISBLANK(C30)),B30&amp;"_"&amp;C30,B30)</f>
+        <v>RAS24</v>
+      </c>
+      <c r="E30" s="1">
         <v>44862</v>
       </c>
-      <c r="C30" s="1">
+      <c r="F30" s="1">
         <v>44867</v>
       </c>
-      <c r="D30" t="s">
+      <c r="G30" t="s">
         <v>31</v>
-      </c>
-      <c r="E30" t="s">
-        <v>69</v>
-      </c>
-      <c r="G30" t="s">
-        <v>69</v>
       </c>
       <c r="H30">
         <v>1</v>
@@ -2169,25 +2367,32 @@
       <c r="U30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V30">
+        <v>1</v>
+      </c>
+      <c r="W30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>70</v>
       </c>
-      <c r="B31" s="1">
+      <c r="B31" t="s">
+        <v>71</v>
+      </c>
+      <c r="D31" t="str">
+        <f>IF(NOT(ISBLANK(C31)),B31&amp;"_"&amp;C31,B31)</f>
+        <v>OPT0024</v>
+      </c>
+      <c r="E31" s="1">
         <v>44911</v>
       </c>
-      <c r="C31" s="1">
+      <c r="F31" s="1">
         <v>44916</v>
       </c>
-      <c r="D31" t="s">
+      <c r="G31" t="s">
         <v>31</v>
-      </c>
-      <c r="E31" t="s">
-        <v>71</v>
-      </c>
-      <c r="G31" t="s">
-        <v>71</v>
       </c>
       <c r="H31">
         <v>0</v>
@@ -2202,7 +2407,7 @@
         <v>11</v>
       </c>
       <c r="M31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N31">
         <v>2</v>
@@ -2222,25 +2427,32 @@
       <c r="U31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V31">
+        <v>1</v>
+      </c>
+      <c r="W31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>70</v>
       </c>
-      <c r="B32" s="1">
+      <c r="B32" t="s">
+        <v>73</v>
+      </c>
+      <c r="D32" t="str">
+        <f>IF(NOT(ISBLANK(C32)),B32&amp;"_"&amp;C32,B32)</f>
+        <v>OPT0030</v>
+      </c>
+      <c r="E32" s="1">
         <v>44911</v>
       </c>
-      <c r="C32" s="1">
+      <c r="F32" s="1">
         <v>44916</v>
       </c>
-      <c r="D32" t="s">
+      <c r="G32" t="s">
         <v>31</v>
-      </c>
-      <c r="E32" t="s">
-        <v>73</v>
-      </c>
-      <c r="G32" t="s">
-        <v>73</v>
       </c>
       <c r="H32">
         <v>0</v>
@@ -2275,25 +2487,32 @@
       <c r="U32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V32">
+        <v>1</v>
+      </c>
+      <c r="W32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>70</v>
       </c>
-      <c r="B33" s="1">
+      <c r="B33" t="s">
+        <v>74</v>
+      </c>
+      <c r="D33" t="str">
+        <f>IF(NOT(ISBLANK(C33)),B33&amp;"_"&amp;C33,B33)</f>
+        <v>OPT0424</v>
+      </c>
+      <c r="E33" s="1">
         <v>44911</v>
       </c>
-      <c r="C33" s="1">
+      <c r="F33" s="1">
         <v>44916</v>
       </c>
-      <c r="D33" t="s">
+      <c r="G33" t="s">
         <v>31</v>
-      </c>
-      <c r="E33" t="s">
-        <v>74</v>
-      </c>
-      <c r="G33" t="s">
-        <v>74</v>
       </c>
       <c r="H33">
         <v>0</v>
@@ -2328,26 +2547,33 @@
       <c r="U33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V33">
+        <v>1</v>
+      </c>
+      <c r="W33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>88</v>
-      </c>
-      <c r="B34" s="1">
+        <v>82</v>
+      </c>
+      <c r="B34" t="s">
+        <v>75</v>
+      </c>
+      <c r="D34" t="str">
+        <f>IF(NOT(ISBLANK(C34)),B34&amp;"_"&amp;C34,B34)</f>
+        <v>OPT0039</v>
+      </c>
+      <c r="E34" s="1">
         <v>44932</v>
       </c>
-      <c r="C34" s="1">
+      <c r="F34" s="1">
         <v>44937</v>
       </c>
-      <c r="D34" t="s">
+      <c r="G34" t="s">
         <v>31</v>
       </c>
-      <c r="E34" t="s">
-        <v>75</v>
-      </c>
-      <c r="G34" t="s">
-        <v>75</v>
-      </c>
       <c r="H34">
         <v>0</v>
       </c>
@@ -2357,6 +2583,12 @@
       <c r="J34">
         <v>3</v>
       </c>
+      <c r="L34">
+        <v>1</v>
+      </c>
+      <c r="M34">
+        <v>0</v>
+      </c>
       <c r="Q34">
         <v>0</v>
       </c>
@@ -2366,31 +2598,38 @@
       <c r="U34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V34">
+        <v>1</v>
+      </c>
+      <c r="W34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>89</v>
-      </c>
-      <c r="B35" s="1">
+        <v>82</v>
+      </c>
+      <c r="B35" t="s">
+        <v>74</v>
+      </c>
+      <c r="D35" t="str">
+        <f>IF(NOT(ISBLANK(C35)),B35&amp;"_"&amp;C35,B35)</f>
+        <v>OPT0424</v>
+      </c>
+      <c r="E35" s="1">
         <v>44932</v>
       </c>
-      <c r="C35" s="1">
+      <c r="F35" s="1">
         <v>44937</v>
       </c>
-      <c r="D35" t="s">
+      <c r="G35" t="s">
         <v>31</v>
       </c>
-      <c r="E35" t="s">
-        <v>71</v>
-      </c>
-      <c r="G35" t="s">
-        <v>71</v>
-      </c>
       <c r="H35">
         <v>0</v>
       </c>
       <c r="I35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J35">
         <v>2</v>
@@ -2398,6 +2637,12 @@
       <c r="K35" t="s">
         <v>76</v>
       </c>
+      <c r="L35">
+        <v>15</v>
+      </c>
+      <c r="M35">
+        <v>1</v>
+      </c>
       <c r="Q35">
         <v>0</v>
       </c>
@@ -2407,25 +2652,35 @@
       <c r="U35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V35">
+        <v>1</v>
+      </c>
+      <c r="W35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>88</v>
-      </c>
-      <c r="B36" s="1">
+        <v>82</v>
+      </c>
+      <c r="B36" t="s">
+        <v>74</v>
+      </c>
+      <c r="C36" t="s">
+        <v>78</v>
+      </c>
+      <c r="D36" t="str">
+        <f>IF(NOT(ISBLANK(C36)),B36&amp;"_"&amp;C36,B36)</f>
+        <v>OPT0424_WNT_high</v>
+      </c>
+      <c r="E36" s="1">
         <v>44932</v>
       </c>
-      <c r="C36" s="1">
+      <c r="F36" s="1">
         <v>44937</v>
       </c>
-      <c r="D36" t="s">
-        <v>31</v>
-      </c>
-      <c r="E36" t="s">
-        <v>74</v>
-      </c>
       <c r="G36" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="H36">
         <v>0</v>
@@ -2439,35 +2694,39 @@
       <c r="K36" t="s">
         <v>76</v>
       </c>
+      <c r="L36">
+        <v>11</v>
+      </c>
+      <c r="M36">
+        <v>1</v>
+      </c>
       <c r="Q36">
         <v>0</v>
       </c>
-      <c r="T36">
-        <v>0</v>
-      </c>
-      <c r="U36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>89</v>
-      </c>
-      <c r="B37" s="1">
+        <v>82</v>
+      </c>
+      <c r="B37" t="s">
+        <v>74</v>
+      </c>
+      <c r="C37" t="s">
+        <v>79</v>
+      </c>
+      <c r="D37" t="str">
+        <f>IF(NOT(ISBLANK(C37)),B37&amp;"_"&amp;C37,B37)</f>
+        <v>OPT0424_WNT_low</v>
+      </c>
+      <c r="E37" s="1">
         <v>44932</v>
       </c>
-      <c r="C37" s="1">
+      <c r="F37" s="1">
         <v>44937</v>
       </c>
-      <c r="D37" t="s">
+      <c r="G37" t="s">
         <v>77</v>
       </c>
-      <c r="E37" t="s">
-        <v>73</v>
-      </c>
-      <c r="G37" t="s">
-        <v>73</v>
-      </c>
       <c r="H37">
         <v>0</v>
       </c>
@@ -2475,121 +2734,142 @@
         <v>0</v>
       </c>
       <c r="J37">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="K37" t="s">
+        <v>76</v>
+      </c>
+      <c r="L37">
+        <v>9</v>
+      </c>
+      <c r="M37">
+        <v>1</v>
       </c>
       <c r="Q37">
         <v>0</v>
       </c>
-      <c r="T37">
-        <v>0</v>
-      </c>
-      <c r="U37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>89</v>
-      </c>
-      <c r="B38" s="1">
+        <v>83</v>
+      </c>
+      <c r="B38" t="s">
+        <v>71</v>
+      </c>
+      <c r="D38" t="str">
+        <f>IF(NOT(ISBLANK(C38)),B38&amp;"_"&amp;C38,B38)</f>
+        <v>OPT0024</v>
+      </c>
+      <c r="E38" s="1">
         <v>44932</v>
       </c>
-      <c r="C38" s="1">
+      <c r="F38" s="1">
         <v>44937</v>
       </c>
-      <c r="D38" t="s">
+      <c r="G38" t="s">
+        <v>31</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <v>1</v>
+      </c>
+      <c r="J38">
+        <v>2</v>
+      </c>
+      <c r="K38" t="s">
+        <v>76</v>
+      </c>
+      <c r="L38">
+        <v>1</v>
+      </c>
+      <c r="M38">
+        <v>0</v>
+      </c>
+      <c r="Q38">
+        <v>0</v>
+      </c>
+      <c r="T38">
+        <v>0</v>
+      </c>
+      <c r="U38">
+        <v>0</v>
+      </c>
+      <c r="V38">
+        <v>1</v>
+      </c>
+      <c r="W38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>83</v>
+      </c>
+      <c r="B39" t="s">
+        <v>71</v>
+      </c>
+      <c r="C39" t="s">
+        <v>78</v>
+      </c>
+      <c r="D39" t="str">
+        <f>IF(NOT(ISBLANK(C39)),B39&amp;"_"&amp;C39,B39)</f>
+        <v>OPT0024_WNT_high</v>
+      </c>
+      <c r="E39" s="1">
+        <v>44932</v>
+      </c>
+      <c r="F39" s="1">
+        <v>44937</v>
+      </c>
+      <c r="G39" t="s">
         <v>77</v>
       </c>
-      <c r="E38" t="s">
-        <v>73</v>
-      </c>
-      <c r="F38" t="s">
-        <v>78</v>
-      </c>
-      <c r="G38" t="s">
+      <c r="H39">
+        <v>0</v>
+      </c>
+      <c r="I39">
+        <v>1</v>
+      </c>
+      <c r="J39">
+        <v>2</v>
+      </c>
+      <c r="K39" t="s">
+        <v>76</v>
+      </c>
+      <c r="L39">
+        <v>5</v>
+      </c>
+      <c r="M39">
+        <v>0</v>
+      </c>
+      <c r="Q39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>83</v>
+      </c>
+      <c r="B40" t="s">
+        <v>71</v>
+      </c>
+      <c r="C40" t="s">
         <v>79</v>
       </c>
-      <c r="H38">
-        <v>0</v>
-      </c>
-      <c r="I38">
-        <v>0</v>
-      </c>
-      <c r="J38">
-        <v>3</v>
-      </c>
-      <c r="Q38">
-        <v>0</v>
-      </c>
-      <c r="T38">
-        <v>0</v>
-      </c>
-      <c r="U38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>89</v>
-      </c>
-      <c r="B39" s="1">
+      <c r="D40" t="str">
+        <f>IF(NOT(ISBLANK(C40)),B40&amp;"_"&amp;C40,B40)</f>
+        <v>OPT0024_WNT_low</v>
+      </c>
+      <c r="E40" s="1">
         <v>44932</v>
       </c>
-      <c r="C39" s="1">
+      <c r="F40" s="1">
         <v>44937</v>
       </c>
-      <c r="D39" t="s">
+      <c r="G40" t="s">
         <v>77</v>
-      </c>
-      <c r="E39" t="s">
-        <v>73</v>
-      </c>
-      <c r="F39" t="s">
-        <v>80</v>
-      </c>
-      <c r="G39" t="s">
-        <v>81</v>
-      </c>
-      <c r="H39">
-        <v>0</v>
-      </c>
-      <c r="I39">
-        <v>0</v>
-      </c>
-      <c r="J39">
-        <v>3</v>
-      </c>
-      <c r="Q39">
-        <v>0</v>
-      </c>
-      <c r="T39">
-        <v>0</v>
-      </c>
-      <c r="U39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>89</v>
-      </c>
-      <c r="B40" s="1">
-        <v>44932</v>
-      </c>
-      <c r="C40" s="1">
-        <v>44937</v>
-      </c>
-      <c r="D40" t="s">
-        <v>77</v>
-      </c>
-      <c r="E40" t="s">
-        <v>71</v>
-      </c>
-      <c r="F40" t="s">
-        <v>78</v>
-      </c>
-      <c r="G40" t="s">
-        <v>82</v>
       </c>
       <c r="H40">
         <v>0</v>
@@ -2603,175 +2883,170 @@
       <c r="K40" t="s">
         <v>76</v>
       </c>
+      <c r="L40">
+        <v>7</v>
+      </c>
+      <c r="M40">
+        <v>0</v>
+      </c>
       <c r="Q40">
         <v>0</v>
       </c>
-      <c r="T40">
-        <v>0</v>
-      </c>
-      <c r="U40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>89</v>
-      </c>
-      <c r="B41" s="1">
+        <v>83</v>
+      </c>
+      <c r="B41" t="s">
+        <v>73</v>
+      </c>
+      <c r="D41" t="str">
+        <f>IF(NOT(ISBLANK(C41)),B41&amp;"_"&amp;C41,B41)</f>
+        <v>OPT0030</v>
+      </c>
+      <c r="E41" s="1">
         <v>44932</v>
       </c>
-      <c r="C41" s="1">
+      <c r="F41" s="1">
         <v>44937</v>
       </c>
-      <c r="D41" t="s">
+      <c r="G41" t="s">
         <v>77</v>
       </c>
-      <c r="E41" t="s">
-        <v>71</v>
-      </c>
-      <c r="F41" t="s">
-        <v>80</v>
-      </c>
-      <c r="G41" t="s">
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
+      </c>
+      <c r="J41">
+        <v>3</v>
+      </c>
+      <c r="L41">
+        <v>15</v>
+      </c>
+      <c r="M41">
+        <v>1</v>
+      </c>
+      <c r="Q41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>83</v>
       </c>
-      <c r="H41">
-        <v>0</v>
-      </c>
-      <c r="I41">
-        <v>1</v>
-      </c>
-      <c r="J41">
+      <c r="B42" t="s">
+        <v>73</v>
+      </c>
+      <c r="C42" t="s">
+        <v>78</v>
+      </c>
+      <c r="D42" t="str">
+        <f>IF(NOT(ISBLANK(C42)),B42&amp;"_"&amp;C42,B42)</f>
+        <v>OPT0030_WNT_high</v>
+      </c>
+      <c r="E42" s="1">
+        <v>44932</v>
+      </c>
+      <c r="F42" s="1">
+        <v>44937</v>
+      </c>
+      <c r="G42" t="s">
+        <v>77</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+      <c r="I42">
+        <v>0</v>
+      </c>
+      <c r="J42">
+        <v>3</v>
+      </c>
+      <c r="L42">
+        <v>11</v>
+      </c>
+      <c r="M42">
+        <v>1</v>
+      </c>
+      <c r="Q42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>83</v>
+      </c>
+      <c r="B43" t="s">
+        <v>73</v>
+      </c>
+      <c r="C43" t="s">
+        <v>79</v>
+      </c>
+      <c r="D43" t="str">
+        <f>IF(NOT(ISBLANK(C43)),B43&amp;"_"&amp;C43,B43)</f>
+        <v>OPT0030_WNT_low</v>
+      </c>
+      <c r="E43" s="1">
+        <v>44932</v>
+      </c>
+      <c r="F43" s="1">
+        <v>44937</v>
+      </c>
+      <c r="G43" t="s">
+        <v>77</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
+      <c r="I43">
+        <v>0</v>
+      </c>
+      <c r="J43">
+        <v>3</v>
+      </c>
+      <c r="L43">
+        <v>9</v>
+      </c>
+      <c r="M43">
+        <v>1</v>
+      </c>
+      <c r="Q43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>86</v>
+      </c>
+      <c r="B44" t="s">
+        <v>73</v>
+      </c>
+      <c r="D44" t="str">
+        <f>IF(NOT(ISBLANK(C44)),B44&amp;"_"&amp;C44,B44)</f>
+        <v>OPT0030</v>
+      </c>
+      <c r="E44" s="1">
+        <v>44974</v>
+      </c>
+      <c r="F44" s="1">
+        <v>44979</v>
+      </c>
+      <c r="G44" t="s">
+        <v>87</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+      <c r="I44">
+        <v>0</v>
+      </c>
+      <c r="J44">
         <v>2</v>
       </c>
-      <c r="K41" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q41">
-        <v>0</v>
-      </c>
-      <c r="T41">
-        <v>0</v>
-      </c>
-      <c r="U41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>88</v>
-      </c>
-      <c r="B42" s="1">
-        <v>44932</v>
-      </c>
-      <c r="C42" s="1">
-        <v>44937</v>
-      </c>
-      <c r="D42" t="s">
-        <v>77</v>
-      </c>
-      <c r="E42" t="s">
-        <v>74</v>
-      </c>
-      <c r="F42" t="s">
-        <v>78</v>
-      </c>
-      <c r="G42" t="s">
-        <v>84</v>
-      </c>
-      <c r="H42">
-        <v>0</v>
-      </c>
-      <c r="I42">
-        <v>0</v>
-      </c>
-      <c r="J42">
-        <v>2</v>
-      </c>
-      <c r="K42" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q42">
-        <v>0</v>
-      </c>
-      <c r="T42">
-        <v>0</v>
-      </c>
-      <c r="U42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>88</v>
-      </c>
-      <c r="B43" s="1">
-        <v>44932</v>
-      </c>
-      <c r="C43" s="1">
-        <v>44937</v>
-      </c>
-      <c r="D43" t="s">
-        <v>77</v>
-      </c>
-      <c r="E43" t="s">
-        <v>74</v>
-      </c>
-      <c r="F43" t="s">
-        <v>80</v>
-      </c>
-      <c r="G43" t="s">
-        <v>85</v>
-      </c>
-      <c r="H43">
-        <v>0</v>
-      </c>
-      <c r="I43">
-        <v>0</v>
-      </c>
-      <c r="J43">
-        <v>2</v>
-      </c>
-      <c r="K43" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q43">
-        <v>0</v>
-      </c>
-      <c r="T43">
-        <v>0</v>
-      </c>
-      <c r="U43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+      <c r="K44" t="s">
         <v>90</v>
-      </c>
-      <c r="B44" s="1">
-        <v>44939</v>
-      </c>
-      <c r="C44" s="1">
-        <v>44944</v>
-      </c>
-      <c r="D44" t="s">
-        <v>31</v>
-      </c>
-      <c r="E44" t="s">
-        <v>60</v>
-      </c>
-      <c r="G44" t="s">
-        <v>60</v>
-      </c>
-      <c r="H44">
-        <v>0</v>
-      </c>
-      <c r="I44">
-        <v>1</v>
-      </c>
-      <c r="J44">
-        <v>3</v>
       </c>
       <c r="L44">
         <v>3</v>
@@ -2789,42 +3064,52 @@
         <v>0</v>
       </c>
       <c r="T44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U44">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V44">
+        <v>0</v>
+      </c>
+      <c r="W44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
+        <v>86</v>
+      </c>
+      <c r="B45" t="s">
+        <v>88</v>
+      </c>
+      <c r="D45" t="str">
+        <f>IF(NOT(ISBLANK(C45)),B45&amp;"_"&amp;C45,B45)</f>
+        <v>OPT0421</v>
+      </c>
+      <c r="E45" s="1">
+        <v>44974</v>
+      </c>
+      <c r="F45" s="1">
+        <v>44979</v>
+      </c>
+      <c r="G45" t="s">
+        <v>87</v>
+      </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
+      <c r="I45">
+        <v>1</v>
+      </c>
+      <c r="J45">
+        <v>2</v>
+      </c>
+      <c r="K45" t="s">
         <v>90</v>
       </c>
-      <c r="B45" s="1">
-        <v>44939</v>
-      </c>
-      <c r="C45" s="1">
-        <v>44944</v>
-      </c>
-      <c r="D45" t="s">
-        <v>31</v>
-      </c>
-      <c r="E45" t="s">
-        <v>47</v>
-      </c>
-      <c r="G45" t="s">
-        <v>47</v>
-      </c>
-      <c r="H45">
-        <v>0</v>
-      </c>
-      <c r="I45">
-        <v>1</v>
-      </c>
-      <c r="J45">
-        <v>3</v>
-      </c>
       <c r="L45">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="M45">
         <v>0</v>
@@ -2839,45 +3124,55 @@
         <v>0</v>
       </c>
       <c r="T45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U45">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V45">
+        <v>0</v>
+      </c>
+      <c r="W45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
+        <v>86</v>
+      </c>
+      <c r="B46" t="s">
+        <v>89</v>
+      </c>
+      <c r="D46" t="str">
+        <f>IF(NOT(ISBLANK(C46)),B46&amp;"_"&amp;C46,B46)</f>
+        <v>RAS28</v>
+      </c>
+      <c r="E46" s="1">
+        <v>44974</v>
+      </c>
+      <c r="F46" s="1">
+        <v>44979</v>
+      </c>
+      <c r="G46" t="s">
+        <v>87</v>
+      </c>
+      <c r="H46">
+        <v>1</v>
+      </c>
+      <c r="I46">
+        <v>0</v>
+      </c>
+      <c r="J46">
+        <v>2</v>
+      </c>
+      <c r="K46" t="s">
         <v>90</v>
       </c>
-      <c r="B46" s="1">
-        <v>44939</v>
-      </c>
-      <c r="C46" s="1">
-        <v>44944</v>
-      </c>
-      <c r="D46" t="s">
-        <v>31</v>
-      </c>
-      <c r="E46" t="s">
-        <v>63</v>
-      </c>
-      <c r="G46" t="s">
-        <v>63</v>
-      </c>
-      <c r="H46">
-        <v>1</v>
-      </c>
-      <c r="I46">
-        <v>0</v>
-      </c>
-      <c r="J46">
-        <v>3</v>
-      </c>
       <c r="L46">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="M46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N46">
         <v>3</v>
@@ -2889,42 +3184,52 @@
         <v>0</v>
       </c>
       <c r="T46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U46">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V46">
+        <v>0</v>
+      </c>
+      <c r="W46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>90</v>
-      </c>
-      <c r="B47" s="1">
+        <v>84</v>
+      </c>
+      <c r="B47" t="s">
+        <v>60</v>
+      </c>
+      <c r="C47" t="s">
+        <v>91</v>
+      </c>
+      <c r="D47" t="str">
+        <f>IF(NOT(ISBLANK(C47)),B47&amp;"_"&amp;C47,B47)</f>
+        <v>OPT0034_Demi</v>
+      </c>
+      <c r="E47" s="1">
         <v>44939</v>
       </c>
-      <c r="C47" s="1">
+      <c r="F47" s="1">
         <v>44944</v>
       </c>
-      <c r="D47" t="s">
+      <c r="G47" t="s">
         <v>31</v>
       </c>
-      <c r="E47" t="s">
-        <v>45</v>
-      </c>
-      <c r="G47" t="s">
-        <v>45</v>
-      </c>
       <c r="H47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J47">
         <v>3</v>
       </c>
       <c r="L47">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M47">
         <v>0</v>
@@ -2939,13 +3244,205 @@
         <v>0</v>
       </c>
       <c r="T47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U47">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="V47">
+        <v>1</v>
+      </c>
+      <c r="W47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>84</v>
+      </c>
+      <c r="B48" t="s">
+        <v>47</v>
+      </c>
+      <c r="C48" t="s">
+        <v>91</v>
+      </c>
+      <c r="D48" t="str">
+        <f>IF(NOT(ISBLANK(C48)),B48&amp;"_"&amp;C48,B48)</f>
+        <v>OPT0413_Demi</v>
+      </c>
+      <c r="E48" s="1">
+        <v>44939</v>
+      </c>
+      <c r="F48" s="1">
+        <v>44944</v>
+      </c>
+      <c r="G48" t="s">
+        <v>31</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+      <c r="I48">
+        <v>1</v>
+      </c>
+      <c r="J48">
+        <v>3</v>
+      </c>
+      <c r="L48">
+        <v>1</v>
+      </c>
+      <c r="M48">
+        <v>0</v>
+      </c>
+      <c r="N48">
+        <v>3</v>
+      </c>
+      <c r="O48" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q48">
+        <v>0</v>
+      </c>
+      <c r="T48">
+        <v>1</v>
+      </c>
+      <c r="U48">
+        <v>0</v>
+      </c>
+      <c r="V48">
+        <v>1</v>
+      </c>
+      <c r="W48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>84</v>
+      </c>
+      <c r="B49" t="s">
+        <v>63</v>
+      </c>
+      <c r="C49" t="s">
+        <v>91</v>
+      </c>
+      <c r="D49" t="str">
+        <f>IF(NOT(ISBLANK(C49)),B49&amp;"_"&amp;C49,B49)</f>
+        <v>RAS11_Demi</v>
+      </c>
+      <c r="E49" s="1">
+        <v>44939</v>
+      </c>
+      <c r="F49" s="1">
+        <v>44944</v>
+      </c>
+      <c r="G49" t="s">
+        <v>31</v>
+      </c>
+      <c r="H49">
+        <v>1</v>
+      </c>
+      <c r="I49">
+        <v>0</v>
+      </c>
+      <c r="J49">
+        <v>3</v>
+      </c>
+      <c r="L49">
+        <v>7</v>
+      </c>
+      <c r="M49">
+        <v>0</v>
+      </c>
+      <c r="N49">
+        <v>3</v>
+      </c>
+      <c r="O49" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q49">
+        <v>0</v>
+      </c>
+      <c r="T49">
+        <v>1</v>
+      </c>
+      <c r="U49">
+        <v>0</v>
+      </c>
+      <c r="V49">
+        <v>1</v>
+      </c>
+      <c r="W49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>84</v>
+      </c>
+      <c r="B50" t="s">
+        <v>45</v>
+      </c>
+      <c r="C50" t="s">
+        <v>91</v>
+      </c>
+      <c r="D50" t="str">
+        <f>IF(NOT(ISBLANK(C50)),B50&amp;"_"&amp;C50,B50)</f>
+        <v>RAS27_Demi</v>
+      </c>
+      <c r="E50" s="1">
+        <v>44939</v>
+      </c>
+      <c r="F50" s="1">
+        <v>44944</v>
+      </c>
+      <c r="G50" t="s">
+        <v>31</v>
+      </c>
+      <c r="H50">
+        <v>1</v>
+      </c>
+      <c r="I50">
+        <v>0</v>
+      </c>
+      <c r="J50">
+        <v>3</v>
+      </c>
+      <c r="L50">
+        <v>5</v>
+      </c>
+      <c r="M50">
+        <v>0</v>
+      </c>
+      <c r="N50">
+        <v>3</v>
+      </c>
+      <c r="O50" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q50">
+        <v>0</v>
+      </c>
+      <c r="T50">
+        <v>1</v>
+      </c>
+      <c r="U50">
+        <v>0</v>
+      </c>
+      <c r="V50">
+        <v>1</v>
+      </c>
+      <c r="W50">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:W50" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:W50">
+      <sortCondition ref="A2:A50"/>
+      <sortCondition ref="D2:D50"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed bug that killed excel saves
</commit_message>
<xml_diff>
--- a/resources/Screening_overview.xlsx
+++ b/resources/Screening_overview.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mhuismans/surfdrive/Promotie/12. STRATEGIC/Analyse 2.0/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{391FB2DF-98B3-874F-B214-18CEF08BFB99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED9178E-AF11-5943-BF24-CFEDD570768B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="660" yWindow="860" windowWidth="27700" windowHeight="14800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="640" yWindow="860" windowWidth="27700" windowHeight="14800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet 1'!$A$1:$W$50</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet 1'!$A$1:$X$50</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="96">
   <si>
     <t>STR_ID</t>
   </si>
@@ -321,6 +321,9 @@
   </si>
   <si>
     <t>DMSO_bad</t>
+  </si>
+  <si>
+    <t>Data_processed</t>
   </si>
 </sst>
 </file>
@@ -664,13 +667,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W50"/>
+  <dimension ref="A1:X50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="S29" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="V51" sqref="V51"/>
+      <selection pane="bottomRight" activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -680,7 +683,7 @@
     <col min="7" max="7" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -739,19 +742,22 @@
         <v>80</v>
       </c>
       <c r="T1" t="s">
+        <v>95</v>
+      </c>
+      <c r="U1" t="s">
         <v>81</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>85</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>93</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -759,7 +765,7 @@
         <v>24</v>
       </c>
       <c r="D2" t="str">
-        <f>IF(NOT(ISBLANK(C2)),B2&amp;"_"&amp;C2,B2)</f>
+        <f t="shared" ref="D2:D33" si="0">IF(NOT(ISBLANK(C2)),B2&amp;"_"&amp;C2,B2)</f>
         <v>OPT0016</v>
       </c>
       <c r="E2" s="1">
@@ -786,14 +792,17 @@
       <c r="Q2">
         <v>0</v>
       </c>
-      <c r="U2">
-        <v>0</v>
-      </c>
-      <c r="W2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -801,7 +810,7 @@
         <v>23</v>
       </c>
       <c r="D3" t="str">
-        <f>IF(NOT(ISBLANK(C3)),B3&amp;"_"&amp;C3,B3)</f>
+        <f t="shared" si="0"/>
         <v>OPT0112</v>
       </c>
       <c r="E3" s="1">
@@ -828,14 +837,17 @@
       <c r="Q3">
         <v>0</v>
       </c>
-      <c r="U3">
-        <v>0</v>
-      </c>
-      <c r="W3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="X3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -843,7 +855,7 @@
         <v>20</v>
       </c>
       <c r="D4" t="str">
-        <f>IF(NOT(ISBLANK(C4)),B4&amp;"_"&amp;C4,B4)</f>
+        <f t="shared" si="0"/>
         <v>RAS04</v>
       </c>
       <c r="E4" s="1">
@@ -873,14 +885,17 @@
       <c r="Q4">
         <v>0</v>
       </c>
-      <c r="U4">
-        <v>0</v>
-      </c>
-      <c r="W4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="X4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -888,7 +903,7 @@
         <v>27</v>
       </c>
       <c r="D5" t="str">
-        <f>IF(NOT(ISBLANK(C5)),B5&amp;"_"&amp;C5,B5)</f>
+        <f t="shared" si="0"/>
         <v>OPT0014</v>
       </c>
       <c r="E5" s="1">
@@ -915,14 +930,17 @@
       <c r="Q5">
         <v>0</v>
       </c>
-      <c r="U5">
-        <v>0</v>
-      </c>
-      <c r="W5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="X5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -930,7 +948,7 @@
         <v>26</v>
       </c>
       <c r="D6" t="str">
-        <f>IF(NOT(ISBLANK(C6)),B6&amp;"_"&amp;C6,B6)</f>
+        <f t="shared" si="0"/>
         <v>RAS25</v>
       </c>
       <c r="E6" s="1">
@@ -960,14 +978,17 @@
       <c r="Q6">
         <v>0</v>
       </c>
-      <c r="U6">
-        <v>0</v>
-      </c>
-      <c r="W6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="X6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -975,7 +996,7 @@
         <v>29</v>
       </c>
       <c r="D7" t="str">
-        <f>IF(NOT(ISBLANK(C7)),B7&amp;"_"&amp;C7,B7)</f>
+        <f t="shared" si="0"/>
         <v>RAS21</v>
       </c>
       <c r="E7" s="1">
@@ -1005,14 +1026,17 @@
       <c r="Q7">
         <v>0</v>
       </c>
-      <c r="U7">
-        <v>0</v>
-      </c>
-      <c r="W7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="X7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -1020,7 +1044,7 @@
         <v>32</v>
       </c>
       <c r="D8" t="str">
-        <f>IF(NOT(ISBLANK(C8)),B8&amp;"_"&amp;C8,B8)</f>
+        <f t="shared" si="0"/>
         <v>OPT0015</v>
       </c>
       <c r="E8" s="1">
@@ -1060,7 +1084,7 @@
         <v>1</v>
       </c>
       <c r="U8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V8">
         <v>0</v>
@@ -1068,8 +1092,11 @@
       <c r="W8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -1077,7 +1104,7 @@
         <v>20</v>
       </c>
       <c r="D9" t="str">
-        <f>IF(NOT(ISBLANK(C9)),B9&amp;"_"&amp;C9,B9)</f>
+        <f t="shared" si="0"/>
         <v>RAS04</v>
       </c>
       <c r="E9" s="1">
@@ -1111,19 +1138,22 @@
         <v>1</v>
       </c>
       <c r="T9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U9">
         <v>0</v>
       </c>
       <c r="V9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="X9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -1131,7 +1161,7 @@
         <v>24</v>
       </c>
       <c r="D10" t="str">
-        <f>IF(NOT(ISBLANK(C10)),B10&amp;"_"&amp;C10,B10)</f>
+        <f t="shared" si="0"/>
         <v>OPT0016</v>
       </c>
       <c r="E10" s="1">
@@ -1168,7 +1198,7 @@
         <v>1</v>
       </c>
       <c r="U10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V10">
         <v>0</v>
@@ -1176,8 +1206,11 @@
       <c r="W10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -1185,7 +1218,7 @@
         <v>23</v>
       </c>
       <c r="D11" t="str">
-        <f>IF(NOT(ISBLANK(C11)),B11&amp;"_"&amp;C11,B11)</f>
+        <f t="shared" si="0"/>
         <v>OPT0112</v>
       </c>
       <c r="E11" s="1">
@@ -1219,19 +1252,22 @@
         <v>0</v>
       </c>
       <c r="T11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U11">
         <v>0</v>
       </c>
       <c r="V11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="X11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -1239,7 +1275,7 @@
         <v>26</v>
       </c>
       <c r="D12" t="str">
-        <f>IF(NOT(ISBLANK(C12)),B12&amp;"_"&amp;C12,B12)</f>
+        <f t="shared" si="0"/>
         <v>RAS25</v>
       </c>
       <c r="E12" s="1">
@@ -1276,7 +1312,7 @@
         <v>1</v>
       </c>
       <c r="U12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V12">
         <v>0</v>
@@ -1284,8 +1320,11 @@
       <c r="W12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -1293,7 +1332,7 @@
         <v>27</v>
       </c>
       <c r="D13" t="str">
-        <f>IF(NOT(ISBLANK(C13)),B13&amp;"_"&amp;C13,B13)</f>
+        <f t="shared" si="0"/>
         <v>OPT0014</v>
       </c>
       <c r="E13" s="1">
@@ -1330,7 +1369,7 @@
         <v>1</v>
       </c>
       <c r="U13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V13">
         <v>0</v>
@@ -1338,8 +1377,11 @@
       <c r="W13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -1347,7 +1389,7 @@
         <v>29</v>
       </c>
       <c r="D14" t="str">
-        <f>IF(NOT(ISBLANK(C14)),B14&amp;"_"&amp;C14,B14)</f>
+        <f t="shared" si="0"/>
         <v>RAS21</v>
       </c>
       <c r="E14" s="1">
@@ -1384,7 +1426,7 @@
         <v>1</v>
       </c>
       <c r="U14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V14">
         <v>0</v>
@@ -1392,8 +1434,11 @@
       <c r="W14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -1401,7 +1446,7 @@
         <v>40</v>
       </c>
       <c r="D15" t="str">
-        <f>IF(NOT(ISBLANK(C15)),B15&amp;"_"&amp;C15,B15)</f>
+        <f t="shared" si="0"/>
         <v>HUB-02-C2-89</v>
       </c>
       <c r="E15" s="1">
@@ -1444,7 +1489,7 @@
         <v>1</v>
       </c>
       <c r="U15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V15">
         <v>0</v>
@@ -1452,8 +1497,11 @@
       <c r="W15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -1461,7 +1509,7 @@
         <v>37</v>
       </c>
       <c r="D16" t="str">
-        <f>IF(NOT(ISBLANK(C16)),B16&amp;"_"&amp;C16,B16)</f>
+        <f t="shared" si="0"/>
         <v>OPT0005</v>
       </c>
       <c r="E16" s="1">
@@ -1501,7 +1549,7 @@
         <v>1</v>
       </c>
       <c r="U16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V16">
         <v>0</v>
@@ -1509,8 +1557,11 @@
       <c r="W16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -1518,7 +1569,7 @@
         <v>47</v>
       </c>
       <c r="D17" t="str">
-        <f>IF(NOT(ISBLANK(C17)),B17&amp;"_"&amp;C17,B17)</f>
+        <f t="shared" si="0"/>
         <v>OPT0413</v>
       </c>
       <c r="E17" s="1">
@@ -1564,7 +1615,7 @@
         <v>1</v>
       </c>
       <c r="U17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V17">
         <v>0</v>
@@ -1572,8 +1623,11 @@
       <c r="W17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>43</v>
       </c>
@@ -1581,7 +1635,7 @@
         <v>44</v>
       </c>
       <c r="D18" t="str">
-        <f>IF(NOT(ISBLANK(C18)),B18&amp;"_"&amp;C18,B18)</f>
+        <f t="shared" si="0"/>
         <v>RAS12</v>
       </c>
       <c r="E18" s="1">
@@ -1621,7 +1675,7 @@
         <v>1</v>
       </c>
       <c r="U18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V18">
         <v>0</v>
@@ -1629,8 +1683,11 @@
       <c r="W18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -1638,7 +1695,7 @@
         <v>45</v>
       </c>
       <c r="D19" t="str">
-        <f>IF(NOT(ISBLANK(C19)),B19&amp;"_"&amp;C19,B19)</f>
+        <f t="shared" si="0"/>
         <v>RAS27</v>
       </c>
       <c r="E19" s="1">
@@ -1681,7 +1738,7 @@
         <v>1</v>
       </c>
       <c r="U19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V19">
         <v>0</v>
@@ -1689,8 +1746,11 @@
       <c r="W19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>49</v>
       </c>
@@ -1698,7 +1758,7 @@
         <v>53</v>
       </c>
       <c r="D20" t="str">
-        <f>IF(NOT(ISBLANK(C20)),B20&amp;"_"&amp;C20,B20)</f>
+        <f t="shared" si="0"/>
         <v>OPT0419</v>
       </c>
       <c r="E20" s="1">
@@ -1741,19 +1801,22 @@
         <v>52</v>
       </c>
       <c r="T20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U20">
         <v>0</v>
       </c>
       <c r="V20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>49</v>
       </c>
@@ -1761,7 +1824,7 @@
         <v>50</v>
       </c>
       <c r="D21" t="str">
-        <f>IF(NOT(ISBLANK(C21)),B21&amp;"_"&amp;C21,B21)</f>
+        <f t="shared" si="0"/>
         <v>RAS05</v>
       </c>
       <c r="E21" s="1">
@@ -1804,19 +1867,22 @@
         <v>52</v>
       </c>
       <c r="T21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U21">
         <v>0</v>
       </c>
       <c r="V21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="X21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>54</v>
       </c>
@@ -1824,7 +1890,7 @@
         <v>58</v>
       </c>
       <c r="D22" t="str">
-        <f>IF(NOT(ISBLANK(C22)),B22&amp;"_"&amp;C22,B22)</f>
+        <f t="shared" si="0"/>
         <v>OPT0408</v>
       </c>
       <c r="E22" s="1">
@@ -1867,7 +1933,7 @@
         <v>1</v>
       </c>
       <c r="U22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V22">
         <v>0</v>
@@ -1875,8 +1941,11 @@
       <c r="W22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>54</v>
       </c>
@@ -1884,7 +1953,7 @@
         <v>55</v>
       </c>
       <c r="D23" t="str">
-        <f>IF(NOT(ISBLANK(C23)),B23&amp;"_"&amp;C23,B23)</f>
+        <f t="shared" si="0"/>
         <v>RAS06</v>
       </c>
       <c r="E23" s="1">
@@ -1927,7 +1996,7 @@
         <v>1</v>
       </c>
       <c r="U23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V23">
         <v>0</v>
@@ -1935,8 +2004,11 @@
       <c r="W23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>54</v>
       </c>
@@ -1944,7 +2016,7 @@
         <v>57</v>
       </c>
       <c r="D24" t="str">
-        <f>IF(NOT(ISBLANK(C24)),B24&amp;"_"&amp;C24,B24)</f>
+        <f t="shared" si="0"/>
         <v>RAS13</v>
       </c>
       <c r="E24" s="1">
@@ -1987,7 +2059,7 @@
         <v>1</v>
       </c>
       <c r="U24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V24">
         <v>0</v>
@@ -1995,8 +2067,11 @@
       <c r="W24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>59</v>
       </c>
@@ -2004,7 +2079,7 @@
         <v>60</v>
       </c>
       <c r="D25" t="str">
-        <f>IF(NOT(ISBLANK(C25)),B25&amp;"_"&amp;C25,B25)</f>
+        <f t="shared" si="0"/>
         <v>OPT0034</v>
       </c>
       <c r="E25" s="1">
@@ -2047,19 +2122,22 @@
         <v>0</v>
       </c>
       <c r="T25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U25">
         <v>0</v>
       </c>
       <c r="V25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="X25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>59</v>
       </c>
@@ -2067,7 +2145,7 @@
         <v>63</v>
       </c>
       <c r="D26" t="str">
-        <f>IF(NOT(ISBLANK(C26)),B26&amp;"_"&amp;C26,B26)</f>
+        <f t="shared" si="0"/>
         <v>RAS11</v>
       </c>
       <c r="E26" s="1">
@@ -2110,19 +2188,22 @@
         <v>0</v>
       </c>
       <c r="T26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U26">
         <v>0</v>
       </c>
       <c r="V26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>64</v>
       </c>
@@ -2130,7 +2211,7 @@
         <v>65</v>
       </c>
       <c r="D27" t="str">
-        <f>IF(NOT(ISBLANK(C27)),B27&amp;"_"&amp;C27,B27)</f>
+        <f t="shared" si="0"/>
         <v>OPT0402</v>
       </c>
       <c r="E27" s="1">
@@ -2173,19 +2254,22 @@
         <v>0</v>
       </c>
       <c r="T27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U27">
         <v>0</v>
       </c>
       <c r="V27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="X27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>64</v>
       </c>
@@ -2193,7 +2277,7 @@
         <v>67</v>
       </c>
       <c r="D28" t="str">
-        <f>IF(NOT(ISBLANK(C28)),B28&amp;"_"&amp;C28,B28)</f>
+        <f t="shared" si="0"/>
         <v>RAS16</v>
       </c>
       <c r="E28" s="1">
@@ -2236,19 +2320,22 @@
         <v>0</v>
       </c>
       <c r="T28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U28">
         <v>0</v>
       </c>
       <c r="V28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>64</v>
       </c>
@@ -2256,7 +2343,7 @@
         <v>68</v>
       </c>
       <c r="D29" t="str">
-        <f>IF(NOT(ISBLANK(C29)),B29&amp;"_"&amp;C29,B29)</f>
+        <f t="shared" si="0"/>
         <v>RAS22</v>
       </c>
       <c r="E29" s="1">
@@ -2299,19 +2386,22 @@
         <v>0</v>
       </c>
       <c r="T29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U29">
         <v>0</v>
       </c>
       <c r="V29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="X29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>64</v>
       </c>
@@ -2319,7 +2409,7 @@
         <v>69</v>
       </c>
       <c r="D30" t="str">
-        <f>IF(NOT(ISBLANK(C30)),B30&amp;"_"&amp;C30,B30)</f>
+        <f t="shared" si="0"/>
         <v>RAS24</v>
       </c>
       <c r="E30" s="1">
@@ -2362,19 +2452,22 @@
         <v>0</v>
       </c>
       <c r="T30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U30">
         <v>0</v>
       </c>
       <c r="V30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="X30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>70</v>
       </c>
@@ -2382,7 +2475,7 @@
         <v>71</v>
       </c>
       <c r="D31" t="str">
-        <f>IF(NOT(ISBLANK(C31)),B31&amp;"_"&amp;C31,B31)</f>
+        <f t="shared" si="0"/>
         <v>OPT0024</v>
       </c>
       <c r="E31" s="1">
@@ -2422,19 +2515,22 @@
         <v>0</v>
       </c>
       <c r="T31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U31">
         <v>0</v>
       </c>
       <c r="V31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="X31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>70</v>
       </c>
@@ -2442,7 +2538,7 @@
         <v>73</v>
       </c>
       <c r="D32" t="str">
-        <f>IF(NOT(ISBLANK(C32)),B32&amp;"_"&amp;C32,B32)</f>
+        <f t="shared" si="0"/>
         <v>OPT0030</v>
       </c>
       <c r="E32" s="1">
@@ -2482,19 +2578,22 @@
         <v>0</v>
       </c>
       <c r="T32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U32">
         <v>0</v>
       </c>
       <c r="V32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="X32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>70</v>
       </c>
@@ -2502,7 +2601,7 @@
         <v>74</v>
       </c>
       <c r="D33" t="str">
-        <f>IF(NOT(ISBLANK(C33)),B33&amp;"_"&amp;C33,B33)</f>
+        <f t="shared" si="0"/>
         <v>OPT0424</v>
       </c>
       <c r="E33" s="1">
@@ -2542,19 +2641,22 @@
         <v>0</v>
       </c>
       <c r="T33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U33">
         <v>0</v>
       </c>
       <c r="V33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>82</v>
       </c>
@@ -2562,7 +2664,7 @@
         <v>75</v>
       </c>
       <c r="D34" t="str">
-        <f>IF(NOT(ISBLANK(C34)),B34&amp;"_"&amp;C34,B34)</f>
+        <f t="shared" ref="D34:D65" si="1">IF(NOT(ISBLANK(C34)),B34&amp;"_"&amp;C34,B34)</f>
         <v>OPT0039</v>
       </c>
       <c r="E34" s="1">
@@ -2593,19 +2695,22 @@
         <v>0</v>
       </c>
       <c r="T34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U34">
         <v>0</v>
       </c>
       <c r="V34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="X34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>82</v>
       </c>
@@ -2613,7 +2718,7 @@
         <v>74</v>
       </c>
       <c r="D35" t="str">
-        <f>IF(NOT(ISBLANK(C35)),B35&amp;"_"&amp;C35,B35)</f>
+        <f t="shared" si="1"/>
         <v>OPT0424</v>
       </c>
       <c r="E35" s="1">
@@ -2647,19 +2752,22 @@
         <v>0</v>
       </c>
       <c r="T35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U35">
         <v>0</v>
       </c>
       <c r="V35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="X35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>82</v>
       </c>
@@ -2670,7 +2778,7 @@
         <v>78</v>
       </c>
       <c r="D36" t="str">
-        <f>IF(NOT(ISBLANK(C36)),B36&amp;"_"&amp;C36,B36)</f>
+        <f t="shared" si="1"/>
         <v>OPT0424_WNT_high</v>
       </c>
       <c r="E36" s="1">
@@ -2703,8 +2811,11 @@
       <c r="Q36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="T36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>82</v>
       </c>
@@ -2715,7 +2826,7 @@
         <v>79</v>
       </c>
       <c r="D37" t="str">
-        <f>IF(NOT(ISBLANK(C37)),B37&amp;"_"&amp;C37,B37)</f>
+        <f t="shared" si="1"/>
         <v>OPT0424_WNT_low</v>
       </c>
       <c r="E37" s="1">
@@ -2748,8 +2859,11 @@
       <c r="Q37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="T37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>83</v>
       </c>
@@ -2757,7 +2871,7 @@
         <v>71</v>
       </c>
       <c r="D38" t="str">
-        <f>IF(NOT(ISBLANK(C38)),B38&amp;"_"&amp;C38,B38)</f>
+        <f t="shared" si="1"/>
         <v>OPT0024</v>
       </c>
       <c r="E38" s="1">
@@ -2791,19 +2905,22 @@
         <v>0</v>
       </c>
       <c r="T38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U38">
         <v>0</v>
       </c>
       <c r="V38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W38">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>83</v>
       </c>
@@ -2814,7 +2931,7 @@
         <v>78</v>
       </c>
       <c r="D39" t="str">
-        <f>IF(NOT(ISBLANK(C39)),B39&amp;"_"&amp;C39,B39)</f>
+        <f t="shared" si="1"/>
         <v>OPT0024_WNT_high</v>
       </c>
       <c r="E39" s="1">
@@ -2847,8 +2964,11 @@
       <c r="Q39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="T39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>83</v>
       </c>
@@ -2859,7 +2979,7 @@
         <v>79</v>
       </c>
       <c r="D40" t="str">
-        <f>IF(NOT(ISBLANK(C40)),B40&amp;"_"&amp;C40,B40)</f>
+        <f t="shared" si="1"/>
         <v>OPT0024_WNT_low</v>
       </c>
       <c r="E40" s="1">
@@ -2892,8 +3012,11 @@
       <c r="Q40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="T40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>83</v>
       </c>
@@ -2901,7 +3024,7 @@
         <v>73</v>
       </c>
       <c r="D41" t="str">
-        <f>IF(NOT(ISBLANK(C41)),B41&amp;"_"&amp;C41,B41)</f>
+        <f t="shared" si="1"/>
         <v>OPT0030</v>
       </c>
       <c r="E41" s="1">
@@ -2931,8 +3054,11 @@
       <c r="Q41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="T41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>83</v>
       </c>
@@ -2943,7 +3069,7 @@
         <v>78</v>
       </c>
       <c r="D42" t="str">
-        <f>IF(NOT(ISBLANK(C42)),B42&amp;"_"&amp;C42,B42)</f>
+        <f t="shared" si="1"/>
         <v>OPT0030_WNT_high</v>
       </c>
       <c r="E42" s="1">
@@ -2973,8 +3099,11 @@
       <c r="Q42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="T42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>83</v>
       </c>
@@ -2985,7 +3114,7 @@
         <v>79</v>
       </c>
       <c r="D43" t="str">
-        <f>IF(NOT(ISBLANK(C43)),B43&amp;"_"&amp;C43,B43)</f>
+        <f t="shared" si="1"/>
         <v>OPT0030_WNT_low</v>
       </c>
       <c r="E43" s="1">
@@ -3015,8 +3144,11 @@
       <c r="Q43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="T43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>86</v>
       </c>
@@ -3024,7 +3156,7 @@
         <v>73</v>
       </c>
       <c r="D44" t="str">
-        <f>IF(NOT(ISBLANK(C44)),B44&amp;"_"&amp;C44,B44)</f>
+        <f t="shared" si="1"/>
         <v>OPT0030</v>
       </c>
       <c r="E44" s="1">
@@ -3070,13 +3202,16 @@
         <v>1</v>
       </c>
       <c r="V44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>86</v>
       </c>
@@ -3084,7 +3219,7 @@
         <v>88</v>
       </c>
       <c r="D45" t="str">
-        <f>IF(NOT(ISBLANK(C45)),B45&amp;"_"&amp;C45,B45)</f>
+        <f t="shared" si="1"/>
         <v>OPT0421</v>
       </c>
       <c r="E45" s="1">
@@ -3130,13 +3265,16 @@
         <v>1</v>
       </c>
       <c r="V45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>86</v>
       </c>
@@ -3144,7 +3282,7 @@
         <v>89</v>
       </c>
       <c r="D46" t="str">
-        <f>IF(NOT(ISBLANK(C46)),B46&amp;"_"&amp;C46,B46)</f>
+        <f t="shared" si="1"/>
         <v>RAS28</v>
       </c>
       <c r="E46" s="1">
@@ -3190,13 +3328,16 @@
         <v>1</v>
       </c>
       <c r="V46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>84</v>
       </c>
@@ -3207,7 +3348,7 @@
         <v>91</v>
       </c>
       <c r="D47" t="str">
-        <f>IF(NOT(ISBLANK(C47)),B47&amp;"_"&amp;C47,B47)</f>
+        <f t="shared" si="1"/>
         <v>OPT0034_Demi</v>
       </c>
       <c r="E47" s="1">
@@ -3247,16 +3388,19 @@
         <v>1</v>
       </c>
       <c r="U47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="X47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>84</v>
       </c>
@@ -3267,7 +3411,7 @@
         <v>91</v>
       </c>
       <c r="D48" t="str">
-        <f>IF(NOT(ISBLANK(C48)),B48&amp;"_"&amp;C48,B48)</f>
+        <f t="shared" si="1"/>
         <v>OPT0413_Demi</v>
       </c>
       <c r="E48" s="1">
@@ -3307,16 +3451,19 @@
         <v>1</v>
       </c>
       <c r="U48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="X48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>84</v>
       </c>
@@ -3327,7 +3474,7 @@
         <v>91</v>
       </c>
       <c r="D49" t="str">
-        <f>IF(NOT(ISBLANK(C49)),B49&amp;"_"&amp;C49,B49)</f>
+        <f t="shared" si="1"/>
         <v>RAS11_Demi</v>
       </c>
       <c r="E49" s="1">
@@ -3367,16 +3514,19 @@
         <v>1</v>
       </c>
       <c r="U49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="X49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>84</v>
       </c>
@@ -3387,7 +3537,7 @@
         <v>91</v>
       </c>
       <c r="D50" t="str">
-        <f>IF(NOT(ISBLANK(C50)),B50&amp;"_"&amp;C50,B50)</f>
+        <f t="shared" si="1"/>
         <v>RAS27_Demi</v>
       </c>
       <c r="E50" s="1">
@@ -3427,18 +3577,21 @@
         <v>1</v>
       </c>
       <c r="U50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W50">
+        <v>1</v>
+      </c>
+      <c r="X50">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:W50" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:W50">
+  <autoFilter ref="A1:X50" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:X50">
       <sortCondition ref="A2:A50"/>
       <sortCondition ref="D2:D50"/>
     </sortState>

</xml_diff>

<commit_message>
Added option to process Halfscreen plates
</commit_message>
<xml_diff>
--- a/resources/Screening_overview.xlsx
+++ b/resources/Screening_overview.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mhuismans/surfdrive/Promotie/12. STRATEGIC/Analyse 2.0/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED9178E-AF11-5943-BF24-CFEDD570768B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35E2D323-EBE5-E84B-91BA-31E4F463EF4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="640" yWindow="860" windowWidth="27700" windowHeight="14800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet 1'!$A$1:$X$50</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet 1'!$A$1:$X$55</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="100">
   <si>
     <t>STR_ID</t>
   </si>
@@ -290,9 +290,6 @@
     <t>STR24B</t>
   </si>
   <si>
-    <t>STR27</t>
-  </si>
-  <si>
     <t>Analyse</t>
   </si>
   <si>
@@ -324,6 +321,21 @@
   </si>
   <si>
     <t>Data_processed</t>
+  </si>
+  <si>
+    <t>STR-D1</t>
+  </si>
+  <si>
+    <t>STR-D2</t>
+  </si>
+  <si>
+    <t>WAS OP</t>
+  </si>
+  <si>
+    <t>RASTRIC_SD</t>
+  </si>
+  <si>
+    <t>HalfScreen_inverted.xlsx</t>
   </si>
 </sst>
 </file>
@@ -667,13 +679,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X50"/>
+  <dimension ref="A1:Y56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="F20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T1" sqref="T1"/>
+      <selection pane="bottomRight" activeCell="V35" sqref="V35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -683,7 +695,7 @@
     <col min="7" max="7" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -742,22 +754,25 @@
         <v>80</v>
       </c>
       <c r="T1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="U1" t="s">
         <v>81</v>
       </c>
       <c r="V1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="W1" t="s">
+        <v>92</v>
+      </c>
+      <c r="X1" t="s">
         <v>93</v>
       </c>
-      <c r="X1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -802,7 +817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -847,7 +862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -894,8 +909,11 @@
       <c r="X4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -940,7 +958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -987,8 +1005,11 @@
       <c r="X6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -1035,8 +1056,11 @@
       <c r="X7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -1096,7 +1120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -1114,7 +1138,7 @@
         <v>44746</v>
       </c>
       <c r="G9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -1152,8 +1176,11 @@
       <c r="X9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -1210,7 +1237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -1267,7 +1294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -1323,8 +1350,11 @@
       <c r="X12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -1381,7 +1411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -1437,8 +1467,11 @@
       <c r="X14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -1501,7 +1534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -1561,7 +1594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -1627,7 +1660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>43</v>
       </c>
@@ -1686,8 +1719,11 @@
       <c r="X18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -1738,19 +1774,22 @@
         <v>1</v>
       </c>
       <c r="U19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V19">
         <v>0</v>
       </c>
       <c r="W19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>49</v>
       </c>
@@ -1816,7 +1855,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>49</v>
       </c>
@@ -1879,10 +1918,13 @@
         <v>1</v>
       </c>
       <c r="X21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="Y21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>54</v>
       </c>
@@ -1945,7 +1987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>54</v>
       </c>
@@ -2007,8 +2049,11 @@
       <c r="X23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>54</v>
       </c>
@@ -2070,8 +2115,11 @@
       <c r="X24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>59</v>
       </c>
@@ -2137,7 +2185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>59</v>
       </c>
@@ -2202,8 +2250,11 @@
       <c r="X26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>64</v>
       </c>
@@ -2269,7 +2320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>64</v>
       </c>
@@ -2334,8 +2385,11 @@
       <c r="X28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>64</v>
       </c>
@@ -2398,10 +2452,13 @@
         <v>1</v>
       </c>
       <c r="X29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="Y29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>64</v>
       </c>
@@ -2464,10 +2521,13 @@
         <v>1</v>
       </c>
       <c r="X30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="Y30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>70</v>
       </c>
@@ -2530,7 +2590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>70</v>
       </c>
@@ -2593,7 +2653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>70</v>
       </c>
@@ -2656,7 +2716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>82</v>
       </c>
@@ -2664,7 +2724,7 @@
         <v>75</v>
       </c>
       <c r="D34" t="str">
-        <f t="shared" ref="D34:D65" si="1">IF(NOT(ISBLANK(C34)),B34&amp;"_"&amp;C34,B34)</f>
+        <f t="shared" ref="D34:D54" si="1">IF(NOT(ISBLANK(C34)),B34&amp;"_"&amp;C34,B34)</f>
         <v>OPT0039</v>
       </c>
       <c r="E34" s="1">
@@ -2710,7 +2770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>82</v>
       </c>
@@ -2758,7 +2818,7 @@
         <v>0</v>
       </c>
       <c r="V35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W35">
         <v>1</v>
@@ -2767,7 +2827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>82</v>
       </c>
@@ -2788,7 +2848,7 @@
         <v>44937</v>
       </c>
       <c r="G36" t="s">
-        <v>77</v>
+        <v>99</v>
       </c>
       <c r="H36">
         <v>0</v>
@@ -2812,10 +2872,22 @@
         <v>0</v>
       </c>
       <c r="T36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="U36">
+        <v>0</v>
+      </c>
+      <c r="V36">
+        <v>1</v>
+      </c>
+      <c r="W36">
+        <v>1</v>
+      </c>
+      <c r="X36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>82</v>
       </c>
@@ -2860,10 +2932,22 @@
         <v>0</v>
       </c>
       <c r="T37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="U37">
+        <v>0</v>
+      </c>
+      <c r="V37">
+        <v>1</v>
+      </c>
+      <c r="W37">
+        <v>1</v>
+      </c>
+      <c r="X37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>83</v>
       </c>
@@ -2911,7 +2995,7 @@
         <v>0</v>
       </c>
       <c r="V38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W38">
         <v>1</v>
@@ -2920,7 +3004,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>83</v>
       </c>
@@ -2941,7 +3025,7 @@
         <v>44937</v>
       </c>
       <c r="G39" t="s">
-        <v>77</v>
+        <v>99</v>
       </c>
       <c r="H39">
         <v>0</v>
@@ -2965,10 +3049,22 @@
         <v>0</v>
       </c>
       <c r="T39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="U39">
+        <v>1</v>
+      </c>
+      <c r="V39">
+        <v>1</v>
+      </c>
+      <c r="W39">
+        <v>0</v>
+      </c>
+      <c r="X39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>83</v>
       </c>
@@ -3013,10 +3109,22 @@
         <v>0</v>
       </c>
       <c r="T40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="U40">
+        <v>1</v>
+      </c>
+      <c r="V40">
+        <v>1</v>
+      </c>
+      <c r="W40">
+        <v>0</v>
+      </c>
+      <c r="X40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>83</v>
       </c>
@@ -3034,7 +3142,7 @@
         <v>44937</v>
       </c>
       <c r="G41" t="s">
-        <v>77</v>
+        <v>99</v>
       </c>
       <c r="H41">
         <v>0</v>
@@ -3055,10 +3163,22 @@
         <v>0</v>
       </c>
       <c r="T41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="U41">
+        <v>0</v>
+      </c>
+      <c r="V41">
+        <v>1</v>
+      </c>
+      <c r="W41">
+        <v>1</v>
+      </c>
+      <c r="X41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>83</v>
       </c>
@@ -3079,7 +3199,7 @@
         <v>44937</v>
       </c>
       <c r="G42" t="s">
-        <v>77</v>
+        <v>99</v>
       </c>
       <c r="H42">
         <v>0</v>
@@ -3100,10 +3220,22 @@
         <v>0</v>
       </c>
       <c r="T42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="U42">
+        <v>0</v>
+      </c>
+      <c r="V42">
+        <v>1</v>
+      </c>
+      <c r="W42">
+        <v>1</v>
+      </c>
+      <c r="X42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>83</v>
       </c>
@@ -3145,12 +3277,24 @@
         <v>0</v>
       </c>
       <c r="T43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="U43">
+        <v>0</v>
+      </c>
+      <c r="V43">
+        <v>1</v>
+      </c>
+      <c r="W43">
+        <v>1</v>
+      </c>
+      <c r="X43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B44" t="s">
         <v>73</v>
@@ -3166,7 +3310,7 @@
         <v>44979</v>
       </c>
       <c r="G44" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H44">
         <v>0</v>
@@ -3178,7 +3322,7 @@
         <v>2</v>
       </c>
       <c r="K44" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L44">
         <v>3</v>
@@ -3202,7 +3346,7 @@
         <v>1</v>
       </c>
       <c r="V44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W44">
         <v>0</v>
@@ -3211,12 +3355,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B45" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D45" t="str">
         <f t="shared" si="1"/>
@@ -3229,7 +3373,7 @@
         <v>44979</v>
       </c>
       <c r="G45" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H45">
         <v>0</v>
@@ -3241,7 +3385,7 @@
         <v>2</v>
       </c>
       <c r="K45" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L45">
         <v>7</v>
@@ -3265,7 +3409,7 @@
         <v>1</v>
       </c>
       <c r="V45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W45">
         <v>0</v>
@@ -3274,12 +3418,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B46" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D46" t="str">
         <f t="shared" si="1"/>
@@ -3292,7 +3436,7 @@
         <v>44979</v>
       </c>
       <c r="G46" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H46">
         <v>1</v>
@@ -3304,7 +3448,7 @@
         <v>2</v>
       </c>
       <c r="K46" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L46">
         <v>13</v>
@@ -3328,7 +3472,7 @@
         <v>1</v>
       </c>
       <c r="V46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W46">
         <v>0</v>
@@ -3336,16 +3480,19 @@
       <c r="X46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="B47" t="s">
         <v>60</v>
       </c>
       <c r="C47" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D47" t="str">
         <f t="shared" si="1"/>
@@ -3400,15 +3547,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="B48" t="s">
         <v>47</v>
       </c>
       <c r="C48" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D48" t="str">
         <f t="shared" si="1"/>
@@ -3457,21 +3604,21 @@
         <v>0</v>
       </c>
       <c r="W48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X48">
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="B49" t="s">
         <v>63</v>
       </c>
       <c r="C49" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D49" t="str">
         <f t="shared" si="1"/>
@@ -3520,21 +3667,24 @@
         <v>0</v>
       </c>
       <c r="W49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="Y49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="B50" t="s">
         <v>45</v>
       </c>
       <c r="C50" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D50" t="str">
         <f t="shared" si="1"/>
@@ -3583,14 +3733,347 @@
         <v>0</v>
       </c>
       <c r="W50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X50">
         <v>0</v>
       </c>
+      <c r="Y50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>96</v>
+      </c>
+      <c r="B51" t="s">
+        <v>53</v>
+      </c>
+      <c r="C51" t="s">
+        <v>90</v>
+      </c>
+      <c r="D51" t="str">
+        <f t="shared" si="1"/>
+        <v>OPT0419_Demi</v>
+      </c>
+      <c r="E51" s="1">
+        <v>44988</v>
+      </c>
+      <c r="F51" s="1">
+        <v>44993</v>
+      </c>
+      <c r="G51" t="s">
+        <v>86</v>
+      </c>
+      <c r="H51">
+        <v>0</v>
+      </c>
+      <c r="I51">
+        <v>1</v>
+      </c>
+      <c r="J51">
+        <v>3</v>
+      </c>
+      <c r="L51">
+        <v>1</v>
+      </c>
+      <c r="M51">
+        <v>0</v>
+      </c>
+      <c r="N51">
+        <v>3</v>
+      </c>
+      <c r="O51" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q51">
+        <v>0</v>
+      </c>
+      <c r="T51">
+        <v>1</v>
+      </c>
+      <c r="U51">
+        <v>1</v>
+      </c>
+      <c r="V51">
+        <v>0</v>
+      </c>
+      <c r="W51">
+        <v>0</v>
+      </c>
+      <c r="X51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>96</v>
+      </c>
+      <c r="B52" t="s">
+        <v>50</v>
+      </c>
+      <c r="C52" t="s">
+        <v>90</v>
+      </c>
+      <c r="D52" t="str">
+        <f t="shared" si="1"/>
+        <v>RAS05_Demi</v>
+      </c>
+      <c r="E52" s="1">
+        <v>44988</v>
+      </c>
+      <c r="F52" s="1">
+        <v>44993</v>
+      </c>
+      <c r="G52" t="s">
+        <v>86</v>
+      </c>
+      <c r="H52">
+        <v>1</v>
+      </c>
+      <c r="I52">
+        <v>0</v>
+      </c>
+      <c r="J52">
+        <v>3</v>
+      </c>
+      <c r="L52">
+        <v>3</v>
+      </c>
+      <c r="M52">
+        <v>0</v>
+      </c>
+      <c r="N52">
+        <v>3</v>
+      </c>
+      <c r="O52" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q52">
+        <v>0</v>
+      </c>
+      <c r="T52">
+        <v>1</v>
+      </c>
+      <c r="U52">
+        <v>1</v>
+      </c>
+      <c r="V52">
+        <v>0</v>
+      </c>
+      <c r="W52">
+        <v>0</v>
+      </c>
+      <c r="X52">
+        <v>0</v>
+      </c>
+      <c r="Y52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>96</v>
+      </c>
+      <c r="B53" t="s">
+        <v>67</v>
+      </c>
+      <c r="C53" t="s">
+        <v>90</v>
+      </c>
+      <c r="D53" t="str">
+        <f t="shared" si="1"/>
+        <v>RAS16_Demi</v>
+      </c>
+      <c r="E53" s="1">
+        <v>44988</v>
+      </c>
+      <c r="F53" s="1">
+        <v>44993</v>
+      </c>
+      <c r="G53" t="s">
+        <v>86</v>
+      </c>
+      <c r="H53">
+        <v>1</v>
+      </c>
+      <c r="I53">
+        <v>0</v>
+      </c>
+      <c r="J53">
+        <v>3</v>
+      </c>
+      <c r="L53">
+        <v>5</v>
+      </c>
+      <c r="M53">
+        <v>0</v>
+      </c>
+      <c r="N53">
+        <v>3</v>
+      </c>
+      <c r="O53" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q53">
+        <v>0</v>
+      </c>
+      <c r="T53">
+        <v>1</v>
+      </c>
+      <c r="U53">
+        <v>1</v>
+      </c>
+      <c r="V53">
+        <v>0</v>
+      </c>
+      <c r="W53">
+        <v>0</v>
+      </c>
+      <c r="X53">
+        <v>0</v>
+      </c>
+      <c r="Y53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>96</v>
+      </c>
+      <c r="B54" t="s">
+        <v>68</v>
+      </c>
+      <c r="C54" t="s">
+        <v>90</v>
+      </c>
+      <c r="D54" t="str">
+        <f t="shared" si="1"/>
+        <v>RAS22_Demi</v>
+      </c>
+      <c r="E54" s="1">
+        <v>44988</v>
+      </c>
+      <c r="F54" s="1">
+        <v>44993</v>
+      </c>
+      <c r="G54" t="s">
+        <v>86</v>
+      </c>
+      <c r="H54">
+        <v>1</v>
+      </c>
+      <c r="I54">
+        <v>0</v>
+      </c>
+      <c r="J54">
+        <v>3</v>
+      </c>
+      <c r="L54">
+        <v>7</v>
+      </c>
+      <c r="M54">
+        <v>0</v>
+      </c>
+      <c r="N54">
+        <v>3</v>
+      </c>
+      <c r="O54" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q54">
+        <v>0</v>
+      </c>
+      <c r="T54">
+        <v>1</v>
+      </c>
+      <c r="U54">
+        <v>1</v>
+      </c>
+      <c r="V54">
+        <v>0</v>
+      </c>
+      <c r="W54">
+        <v>0</v>
+      </c>
+      <c r="X54">
+        <v>0</v>
+      </c>
+      <c r="Y54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>96</v>
+      </c>
+      <c r="B55" t="s">
+        <v>69</v>
+      </c>
+      <c r="C55" t="s">
+        <v>90</v>
+      </c>
+      <c r="D55" t="str">
+        <f t="shared" ref="D55" si="2">IF(NOT(ISBLANK(C55)),B55&amp;"_"&amp;C55,B55)</f>
+        <v>RAS24_Demi</v>
+      </c>
+      <c r="E55" s="1">
+        <v>44988</v>
+      </c>
+      <c r="F55" s="1">
+        <v>44993</v>
+      </c>
+      <c r="G55" t="s">
+        <v>86</v>
+      </c>
+      <c r="H55">
+        <v>1</v>
+      </c>
+      <c r="I55">
+        <v>0</v>
+      </c>
+      <c r="J55">
+        <v>3</v>
+      </c>
+      <c r="L55">
+        <v>15</v>
+      </c>
+      <c r="M55">
+        <v>1</v>
+      </c>
+      <c r="N55">
+        <v>0</v>
+      </c>
+      <c r="O55" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q55">
+        <v>0</v>
+      </c>
+      <c r="T55">
+        <v>1</v>
+      </c>
+      <c r="U55">
+        <v>0</v>
+      </c>
+      <c r="V55">
+        <v>0</v>
+      </c>
+      <c r="W55">
+        <v>1</v>
+      </c>
+      <c r="X55">
+        <v>1</v>
+      </c>
+      <c r="Y55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="E56" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:X50" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <autoFilter ref="A1:X55" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:X50">
       <sortCondition ref="A2:A50"/>
       <sortCondition ref="D2:D50"/>

</xml_diff>

<commit_message>
made it easier to select for specific conditions to plot
</commit_message>
<xml_diff>
--- a/resources/Screening_overview.xlsx
+++ b/resources/Screening_overview.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mhuismans/surfdrive/Promotie/12. STRATEGIC/Analyse 2.0/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35E2D323-EBE5-E84B-91BA-31E4F463EF4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A90020E-82D4-6D4A-B908-43CC0A40480E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-35700" yWindow="2380" windowWidth="28800" windowHeight="16020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet 1'!$A$1:$X$55</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet 1'!$A$1:$Y$55</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="101">
   <si>
     <t>STR_ID</t>
   </si>
@@ -336,6 +336,9 @@
   </si>
   <si>
     <t>HalfScreen_inverted.xlsx</t>
+  </si>
+  <si>
+    <t>Analyse2</t>
   </si>
 </sst>
 </file>
@@ -679,13 +682,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y56"/>
+  <dimension ref="A1:Z56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="F20" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="J23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="V35" sqref="V35"/>
+      <selection pane="bottomRight" activeCell="V45" sqref="V45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -695,7 +698,7 @@
     <col min="7" max="7" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -763,16 +766,19 @@
         <v>84</v>
       </c>
       <c r="W1" t="s">
+        <v>100</v>
+      </c>
+      <c r="X1" t="s">
         <v>92</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>93</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -813,11 +819,14 @@
       <c r="V2">
         <v>0</v>
       </c>
-      <c r="X2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -858,11 +867,14 @@
       <c r="V3">
         <v>0</v>
       </c>
-      <c r="X3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="W3">
+        <v>0</v>
+      </c>
+      <c r="Y3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -906,14 +918,17 @@
       <c r="V4">
         <v>0</v>
       </c>
-      <c r="X4">
-        <v>1</v>
+      <c r="W4">
+        <v>0</v>
       </c>
       <c r="Y4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="Z4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -954,11 +969,14 @@
       <c r="V5">
         <v>0</v>
       </c>
-      <c r="X5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="Y5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -1002,14 +1020,17 @@
       <c r="V6">
         <v>0</v>
       </c>
-      <c r="X6">
-        <v>1</v>
+      <c r="W6">
+        <v>0</v>
       </c>
       <c r="Y6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="Z6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -1053,14 +1074,17 @@
       <c r="V7">
         <v>0</v>
       </c>
-      <c r="X7">
-        <v>1</v>
+      <c r="W7">
+        <v>0</v>
       </c>
       <c r="Y7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="Z7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -1119,8 +1143,11 @@
       <c r="X8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Y8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -1171,16 +1198,19 @@
         <v>0</v>
       </c>
       <c r="W9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -1236,8 +1266,11 @@
       <c r="X10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Y10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -1288,13 +1321,16 @@
         <v>0</v>
       </c>
       <c r="W11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="Y11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -1353,8 +1389,11 @@
       <c r="Y12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -1410,8 +1449,11 @@
       <c r="X13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Y13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -1470,8 +1512,11 @@
       <c r="Y14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -1533,8 +1578,11 @@
       <c r="X15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Y15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -1593,8 +1641,11 @@
       <c r="X16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Y16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -1659,8 +1710,11 @@
       <c r="X17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Y17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>43</v>
       </c>
@@ -1722,8 +1776,11 @@
       <c r="Y18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -1780,16 +1837,19 @@
         <v>0</v>
       </c>
       <c r="W19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>49</v>
       </c>
@@ -1849,13 +1909,16 @@
         <v>0</v>
       </c>
       <c r="W20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Y20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>49</v>
       </c>
@@ -1915,16 +1978,19 @@
         <v>0</v>
       </c>
       <c r="W21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X21">
         <v>1</v>
       </c>
       <c r="Y21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="Z21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>54</v>
       </c>
@@ -1986,8 +2052,11 @@
       <c r="X22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Y22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>54</v>
       </c>
@@ -2052,8 +2121,11 @@
       <c r="Y23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>54</v>
       </c>
@@ -2118,8 +2190,11 @@
       <c r="Y24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>59</v>
       </c>
@@ -2179,13 +2254,16 @@
         <v>0</v>
       </c>
       <c r="W25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="Y25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>59</v>
       </c>
@@ -2245,7 +2323,7 @@
         <v>0</v>
       </c>
       <c r="W26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X26">
         <v>1</v>
@@ -2253,8 +2331,11 @@
       <c r="Y26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>64</v>
       </c>
@@ -2314,13 +2395,16 @@
         <v>0</v>
       </c>
       <c r="W27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="Y27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>64</v>
       </c>
@@ -2380,7 +2464,7 @@
         <v>0</v>
       </c>
       <c r="W28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X28">
         <v>1</v>
@@ -2388,8 +2472,11 @@
       <c r="Y28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>64</v>
       </c>
@@ -2449,16 +2536,19 @@
         <v>0</v>
       </c>
       <c r="W29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X29">
         <v>1</v>
       </c>
       <c r="Y29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="Z29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>64</v>
       </c>
@@ -2518,7 +2608,7 @@
         <v>0</v>
       </c>
       <c r="W30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X30">
         <v>1</v>
@@ -2526,8 +2616,11 @@
       <c r="Y30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>70</v>
       </c>
@@ -2584,13 +2677,16 @@
         <v>0</v>
       </c>
       <c r="W31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="Y31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>70</v>
       </c>
@@ -2647,13 +2743,16 @@
         <v>0</v>
       </c>
       <c r="W32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="Y32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>70</v>
       </c>
@@ -2710,13 +2809,16 @@
         <v>0</v>
       </c>
       <c r="W33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Y33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>82</v>
       </c>
@@ -2764,13 +2866,16 @@
         <v>0</v>
       </c>
       <c r="W34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="Y34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>82</v>
       </c>
@@ -2818,16 +2923,19 @@
         <v>0</v>
       </c>
       <c r="V35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="Y35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>82</v>
       </c>
@@ -2878,16 +2986,19 @@
         <v>0</v>
       </c>
       <c r="V36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Y36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>82</v>
       </c>
@@ -2938,16 +3049,19 @@
         <v>0</v>
       </c>
       <c r="V37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X37">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Y37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>83</v>
       </c>
@@ -2995,16 +3109,19 @@
         <v>0</v>
       </c>
       <c r="V38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X38">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Y38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>83</v>
       </c>
@@ -3058,13 +3175,16 @@
         <v>1</v>
       </c>
       <c r="W39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Y39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>83</v>
       </c>
@@ -3118,13 +3238,16 @@
         <v>1</v>
       </c>
       <c r="W40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Y40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>83</v>
       </c>
@@ -3169,16 +3292,19 @@
         <v>0</v>
       </c>
       <c r="V41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X41">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Y41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>83</v>
       </c>
@@ -3229,13 +3355,16 @@
         <v>1</v>
       </c>
       <c r="W42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="Y42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>83</v>
       </c>
@@ -3286,13 +3415,16 @@
         <v>1</v>
       </c>
       <c r="W43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="Y43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>85</v>
       </c>
@@ -3354,8 +3486,11 @@
       <c r="X44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Y44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>85</v>
       </c>
@@ -3417,8 +3552,11 @@
       <c r="X45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Y45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>85</v>
       </c>
@@ -3483,8 +3621,11 @@
       <c r="Y46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>95</v>
       </c>
@@ -3541,13 +3682,16 @@
         <v>0</v>
       </c>
       <c r="W47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="Y47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>95</v>
       </c>
@@ -3609,8 +3753,11 @@
       <c r="X48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Y48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>95</v>
       </c>
@@ -3673,10 +3820,13 @@
         <v>0</v>
       </c>
       <c r="Y49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="Z49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>95</v>
       </c>
@@ -3741,8 +3891,11 @@
       <c r="Y50">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>96</v>
       </c>
@@ -3804,8 +3957,11 @@
       <c r="X51">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Y51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>96</v>
       </c>
@@ -3870,8 +4026,11 @@
       <c r="Y52">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>96</v>
       </c>
@@ -3934,10 +4093,13 @@
         <v>0</v>
       </c>
       <c r="Y53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="Z53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>96</v>
       </c>
@@ -4002,8 +4164,11 @@
       <c r="Y54">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>96</v>
       </c>
@@ -4060,7 +4225,7 @@
         <v>0</v>
       </c>
       <c r="W55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X55">
         <v>1</v>
@@ -4068,13 +4233,16 @@
       <c r="Y55">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Z55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:26" x14ac:dyDescent="0.2">
       <c r="E56" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:X55" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:X50">
+  <autoFilter ref="A1:Y55" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Y50">
       <sortCondition ref="A2:A50"/>
       <sortCondition ref="D2:D50"/>
     </sortState>

</xml_diff>

<commit_message>
Script3 aangepast om numerieke variabelen te plotten
</commit_message>
<xml_diff>
--- a/resources/Screening_overview.xlsx
+++ b/resources/Screening_overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mhuismans/surfdrive/Promotie/12. STRATEGIC/Analyse 2.0/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A90020E-82D4-6D4A-B908-43CC0A40480E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD32BCE4-A185-7E4D-915D-11C510436C35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35700" yWindow="2380" windowWidth="28800" windowHeight="16020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="102">
   <si>
     <t>STR_ID</t>
   </si>
@@ -332,13 +332,16 @@
     <t>WAS OP</t>
   </si>
   <si>
-    <t>RASTRIC_SD</t>
-  </si>
-  <si>
     <t>HalfScreen_inverted.xlsx</t>
   </si>
   <si>
     <t>Analyse2</t>
+  </si>
+  <si>
+    <t>Clin_benefit</t>
+  </si>
+  <si>
+    <t>RAS_pct_change</t>
   </si>
 </sst>
 </file>
@@ -383,9 +386,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -682,13 +686,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z56"/>
+  <dimension ref="A1:AA56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="J23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="V45" sqref="V45"/>
+      <selection pane="bottomRight" activeCell="AA54" sqref="AA54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -696,9 +700,14 @@
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="18" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.33203125" customWidth="1"/>
+    <col min="11" max="11" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="64.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -766,7 +775,7 @@
         <v>84</v>
       </c>
       <c r="W1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="X1" t="s">
         <v>92</v>
@@ -775,10 +784,13 @@
         <v>93</v>
       </c>
       <c r="Z1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -826,7 +838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -874,7 +886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -927,8 +939,11 @@
       <c r="Z4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA4" s="2">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -976,7 +991,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -1029,8 +1044,11 @@
       <c r="Z6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA6" s="2">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -1083,17 +1101,20 @@
       <c r="Z7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA7" s="2">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>30</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="0"/>
-        <v>OPT0015</v>
+        <v>RAS04</v>
       </c>
       <c r="E8" s="1">
         <v>44741</v>
@@ -1102,37 +1123,34 @@
         <v>44746</v>
       </c>
       <c r="G8" t="s">
-        <v>31</v>
+        <v>91</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L8">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="M8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O8" t="s">
         <v>21</v>
       </c>
-      <c r="P8" t="s">
-        <v>33</v>
-      </c>
       <c r="Q8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T8">
         <v>1</v>
       </c>
       <c r="U8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V8">
         <v>0</v>
@@ -1141,22 +1159,28 @@
         <v>0</v>
       </c>
       <c r="X8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="Z8">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="2">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" si="0"/>
-        <v>RAS04</v>
+        <v>OPT0015</v>
       </c>
       <c r="E9" s="1">
         <v>44741</v>
@@ -1165,34 +1189,37 @@
         <v>44746</v>
       </c>
       <c r="G9" t="s">
-        <v>91</v>
+        <v>31</v>
       </c>
       <c r="H9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L9">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="M9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O9" t="s">
         <v>21</v>
       </c>
+      <c r="P9" t="s">
+        <v>33</v>
+      </c>
       <c r="Q9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T9">
         <v>1</v>
       </c>
       <c r="U9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V9">
         <v>0</v>
@@ -1201,16 +1228,14 @@
         <v>0</v>
       </c>
       <c r="X9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y9">
         <v>0</v>
       </c>
-      <c r="Z9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA9" s="2"/>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -1270,7 +1295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -1330,7 +1355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -1378,7 +1403,7 @@
         <v>1</v>
       </c>
       <c r="V12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W12">
         <v>0</v>
@@ -1392,8 +1417,11 @@
       <c r="Z12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA12" s="2">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -1453,7 +1481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -1501,7 +1529,7 @@
         <v>1</v>
       </c>
       <c r="V14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W14">
         <v>0</v>
@@ -1515,8 +1543,11 @@
       <c r="Z14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA14" s="2">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -1582,7 +1613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -1645,7 +1676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -1714,7 +1745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>43</v>
       </c>
@@ -1765,7 +1796,7 @@
         <v>1</v>
       </c>
       <c r="V18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W18">
         <v>0</v>
@@ -1779,8 +1810,11 @@
       <c r="Z18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA18" s="2">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -1848,17 +1882,20 @@
       <c r="Z19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA19" s="2">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>49</v>
       </c>
       <c r="B20" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D20" t="str">
         <f t="shared" si="0"/>
-        <v>OPT0419</v>
+        <v>RAS05</v>
       </c>
       <c r="E20" s="1">
         <v>44823</v>
@@ -1870,19 +1907,19 @@
         <v>31</v>
       </c>
       <c r="H20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J20">
         <v>2</v>
       </c>
       <c r="L20">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="M20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N20">
         <v>2</v>
@@ -1917,17 +1954,23 @@
       <c r="Y20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="Z20">
+        <v>0</v>
+      </c>
+      <c r="AA20" s="2">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>49</v>
       </c>
       <c r="B21" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D21" t="str">
         <f t="shared" si="0"/>
-        <v>RAS05</v>
+        <v>OPT0419</v>
       </c>
       <c r="E21" s="1">
         <v>44823</v>
@@ -1939,19 +1982,19 @@
         <v>31</v>
       </c>
       <c r="H21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J21">
         <v>2</v>
       </c>
       <c r="L21">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="M21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N21">
         <v>2</v>
@@ -1986,20 +2029,18 @@
       <c r="Y21">
         <v>1</v>
       </c>
-      <c r="Z21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA21" s="2"/>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>54</v>
       </c>
       <c r="B22" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D22" t="str">
         <f t="shared" si="0"/>
-        <v>OPT0408</v>
+        <v>RAS06</v>
       </c>
       <c r="E22" s="1">
         <v>44830</v>
@@ -2011,16 +2052,16 @@
         <v>31</v>
       </c>
       <c r="H22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J22">
         <v>3</v>
       </c>
       <c r="L22">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M22">
         <v>0</v>
@@ -2044,7 +2085,7 @@
         <v>1</v>
       </c>
       <c r="V22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W22">
         <v>0</v>
@@ -2055,17 +2096,23 @@
       <c r="Y22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="Z22">
+        <v>0</v>
+      </c>
+      <c r="AA22" s="2">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>54</v>
       </c>
       <c r="B23" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D23" t="str">
         <f t="shared" si="0"/>
-        <v>RAS06</v>
+        <v>RAS13</v>
       </c>
       <c r="E23" s="1">
         <v>44830</v>
@@ -2086,7 +2133,7 @@
         <v>3</v>
       </c>
       <c r="L23">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M23">
         <v>0</v>
@@ -2110,7 +2157,7 @@
         <v>1</v>
       </c>
       <c r="V23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W23">
         <v>0</v>
@@ -2124,17 +2171,20 @@
       <c r="Z23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA23" s="2">
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>54</v>
       </c>
       <c r="B24" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D24" t="str">
         <f t="shared" si="0"/>
-        <v>RAS13</v>
+        <v>OPT0408</v>
       </c>
       <c r="E24" s="1">
         <v>44830</v>
@@ -2146,16 +2196,16 @@
         <v>31</v>
       </c>
       <c r="H24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J24">
         <v>3</v>
       </c>
       <c r="L24">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="M24">
         <v>0</v>
@@ -2190,20 +2240,18 @@
       <c r="Y24">
         <v>0</v>
       </c>
-      <c r="Z24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA24" s="2"/>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>59</v>
       </c>
       <c r="B25" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D25" t="str">
         <f t="shared" si="0"/>
-        <v>OPT0034</v>
+        <v>RAS11</v>
       </c>
       <c r="E25" s="1">
         <v>44841</v>
@@ -2215,10 +2263,10 @@
         <v>31</v>
       </c>
       <c r="H25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J25">
         <v>3</v>
@@ -2227,7 +2275,7 @@
         <v>61</v>
       </c>
       <c r="L25">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="M25">
         <v>0</v>
@@ -2260,19 +2308,25 @@
         <v>1</v>
       </c>
       <c r="Y25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="Z25">
+        <v>1</v>
+      </c>
+      <c r="AA25" s="2">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>59</v>
       </c>
       <c r="B26" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D26" t="str">
         <f t="shared" si="0"/>
-        <v>RAS11</v>
+        <v>OPT0034</v>
       </c>
       <c r="E26" s="1">
         <v>44841</v>
@@ -2284,10 +2338,10 @@
         <v>31</v>
       </c>
       <c r="H26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J26">
         <v>3</v>
@@ -2296,7 +2350,7 @@
         <v>61</v>
       </c>
       <c r="L26">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="M26">
         <v>0</v>
@@ -2329,22 +2383,20 @@
         <v>1</v>
       </c>
       <c r="Y26">
-        <v>1</v>
-      </c>
-      <c r="Z26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="AA26" s="2"/>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>64</v>
       </c>
       <c r="B27" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D27" t="str">
         <f t="shared" si="0"/>
-        <v>OPT0402</v>
+        <v>RAS16</v>
       </c>
       <c r="E27" s="1">
         <v>44862</v>
@@ -2356,10 +2408,10 @@
         <v>31</v>
       </c>
       <c r="H27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J27">
         <v>2</v>
@@ -2368,7 +2420,7 @@
         <v>48</v>
       </c>
       <c r="L27">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="M27">
         <v>1</v>
@@ -2401,19 +2453,25 @@
         <v>1</v>
       </c>
       <c r="Y27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="Z27">
+        <v>0</v>
+      </c>
+      <c r="AA27" s="2">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>64</v>
       </c>
       <c r="B28" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D28" t="str">
         <f t="shared" si="0"/>
-        <v>RAS16</v>
+        <v>OPT0402</v>
       </c>
       <c r="E28" s="1">
         <v>44862</v>
@@ -2425,10 +2483,10 @@
         <v>31</v>
       </c>
       <c r="H28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J28">
         <v>2</v>
@@ -2437,7 +2495,7 @@
         <v>48</v>
       </c>
       <c r="L28">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="M28">
         <v>1</v>
@@ -2470,13 +2528,11 @@
         <v>1</v>
       </c>
       <c r="Y28">
-        <v>1</v>
-      </c>
-      <c r="Z28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="AA28" s="2"/>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>64</v>
       </c>
@@ -2547,8 +2603,11 @@
       <c r="Z29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA29" s="2">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>64</v>
       </c>
@@ -2617,10 +2676,13 @@
         <v>1</v>
       </c>
       <c r="Z30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="AA30" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>70</v>
       </c>
@@ -2686,7 +2748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>70</v>
       </c>
@@ -2752,7 +2814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>70</v>
       </c>
@@ -2818,7 +2880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>82</v>
       </c>
@@ -2826,7 +2888,7 @@
         <v>75</v>
       </c>
       <c r="D34" t="str">
-        <f t="shared" ref="D34:D54" si="1">IF(NOT(ISBLANK(C34)),B34&amp;"_"&amp;C34,B34)</f>
+        <f t="shared" ref="D34:D65" si="1">IF(NOT(ISBLANK(C34)),B34&amp;"_"&amp;C34,B34)</f>
         <v>OPT0039</v>
       </c>
       <c r="E34" s="1">
@@ -2875,7 +2937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>82</v>
       </c>
@@ -2935,7 +2997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>82</v>
       </c>
@@ -2956,7 +3018,7 @@
         <v>44937</v>
       </c>
       <c r="G36" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H36">
         <v>0</v>
@@ -2998,7 +3060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>82</v>
       </c>
@@ -3061,7 +3123,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>83</v>
       </c>
@@ -3121,7 +3183,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>83</v>
       </c>
@@ -3142,7 +3204,7 @@
         <v>44937</v>
       </c>
       <c r="G39" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H39">
         <v>0</v>
@@ -3172,10 +3234,10 @@
         <v>1</v>
       </c>
       <c r="V39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X39">
         <v>0</v>
@@ -3184,7 +3246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>83</v>
       </c>
@@ -3235,10 +3297,10 @@
         <v>1</v>
       </c>
       <c r="V40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X40">
         <v>0</v>
@@ -3247,7 +3309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>83</v>
       </c>
@@ -3265,7 +3327,7 @@
         <v>44937</v>
       </c>
       <c r="G41" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H41">
         <v>0</v>
@@ -3304,7 +3366,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>83</v>
       </c>
@@ -3325,7 +3387,7 @@
         <v>44937</v>
       </c>
       <c r="G42" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H42">
         <v>0</v>
@@ -3352,7 +3414,7 @@
         <v>0</v>
       </c>
       <c r="V42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W42">
         <v>0</v>
@@ -3364,7 +3426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>83</v>
       </c>
@@ -3412,7 +3474,7 @@
         <v>0</v>
       </c>
       <c r="V43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W43">
         <v>0</v>
@@ -3424,40 +3486,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="B44" t="s">
-        <v>73</v>
+        <v>63</v>
+      </c>
+      <c r="C44" t="s">
+        <v>90</v>
       </c>
       <c r="D44" t="str">
         <f t="shared" si="1"/>
-        <v>OPT0030</v>
+        <v>RAS11_Demi</v>
       </c>
       <c r="E44" s="1">
-        <v>44974</v>
+        <v>44939</v>
       </c>
       <c r="F44" s="1">
-        <v>44979</v>
+        <v>44944</v>
       </c>
       <c r="G44" t="s">
-        <v>86</v>
+        <v>31</v>
       </c>
       <c r="H44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I44">
         <v>0</v>
       </c>
       <c r="J44">
-        <v>2</v>
-      </c>
-      <c r="K44" t="s">
-        <v>89</v>
+        <v>3</v>
       </c>
       <c r="L44">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="M44">
         <v>0</v>
@@ -3478,7 +3540,7 @@
         <v>1</v>
       </c>
       <c r="V44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W44">
         <v>0</v>
@@ -3489,26 +3551,35 @@
       <c r="Y44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="Z44">
+        <v>1</v>
+      </c>
+      <c r="AA44" s="2">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="45" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="B45" t="s">
-        <v>87</v>
+        <v>60</v>
+      </c>
+      <c r="C45" t="s">
+        <v>90</v>
       </c>
       <c r="D45" t="str">
         <f t="shared" si="1"/>
-        <v>OPT0421</v>
+        <v>OPT0034_Demi</v>
       </c>
       <c r="E45" s="1">
-        <v>44974</v>
+        <v>44939</v>
       </c>
       <c r="F45" s="1">
-        <v>44979</v>
+        <v>44944</v>
       </c>
       <c r="G45" t="s">
-        <v>86</v>
+        <v>31</v>
       </c>
       <c r="H45">
         <v>0</v>
@@ -3517,13 +3588,10 @@
         <v>1</v>
       </c>
       <c r="J45">
-        <v>2</v>
-      </c>
-      <c r="K45" t="s">
-        <v>89</v>
+        <v>3</v>
       </c>
       <c r="L45">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="M45">
         <v>0</v>
@@ -3550,49 +3618,49 @@
         <v>0</v>
       </c>
       <c r="X45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y45">
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="B46" t="s">
-        <v>88</v>
+        <v>47</v>
+      </c>
+      <c r="C46" t="s">
+        <v>90</v>
       </c>
       <c r="D46" t="str">
         <f t="shared" si="1"/>
-        <v>RAS28</v>
+        <v>OPT0413_Demi</v>
       </c>
       <c r="E46" s="1">
-        <v>44974</v>
+        <v>44939</v>
       </c>
       <c r="F46" s="1">
-        <v>44979</v>
+        <v>44944</v>
       </c>
       <c r="G46" t="s">
-        <v>86</v>
+        <v>31</v>
       </c>
       <c r="H46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J46">
-        <v>2</v>
-      </c>
-      <c r="K46" t="s">
-        <v>89</v>
+        <v>3</v>
       </c>
       <c r="L46">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="M46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N46">
         <v>3</v>
@@ -3621,23 +3689,21 @@
       <c r="Y46">
         <v>0</v>
       </c>
-      <c r="Z46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA46" s="2"/>
+    </row>
+    <row r="47" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>95</v>
       </c>
       <c r="B47" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="C47" t="s">
         <v>90</v>
       </c>
       <c r="D47" t="str">
         <f t="shared" si="1"/>
-        <v>OPT0034_Demi</v>
+        <v>RAS27_Demi</v>
       </c>
       <c r="E47" s="1">
         <v>44939</v>
@@ -3649,16 +3715,16 @@
         <v>31</v>
       </c>
       <c r="H47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J47">
         <v>3</v>
       </c>
       <c r="L47">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="M47">
         <v>0</v>
@@ -3679,52 +3745,58 @@
         <v>1</v>
       </c>
       <c r="V47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W47">
         <v>0</v>
       </c>
       <c r="X47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y47">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="Z47">
+        <v>0</v>
+      </c>
+      <c r="AA47" s="2">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="48" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="B48" t="s">
-        <v>47</v>
-      </c>
-      <c r="C48" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="D48" t="str">
         <f t="shared" si="1"/>
-        <v>OPT0413_Demi</v>
+        <v>OPT0030</v>
       </c>
       <c r="E48" s="1">
-        <v>44939</v>
+        <v>44974</v>
       </c>
       <c r="F48" s="1">
-        <v>44944</v>
+        <v>44979</v>
       </c>
       <c r="G48" t="s">
-        <v>31</v>
+        <v>86</v>
       </c>
       <c r="H48">
         <v>0</v>
       </c>
       <c r="I48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J48">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="K48" t="s">
+        <v>89</v>
       </c>
       <c r="L48">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M48">
         <v>0</v>
@@ -3757,37 +3829,37 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="B49" t="s">
-        <v>63</v>
-      </c>
-      <c r="C49" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D49" t="str">
         <f t="shared" si="1"/>
-        <v>RAS11_Demi</v>
+        <v>OPT0421</v>
       </c>
       <c r="E49" s="1">
-        <v>44939</v>
+        <v>44974</v>
       </c>
       <c r="F49" s="1">
-        <v>44944</v>
+        <v>44979</v>
       </c>
       <c r="G49" t="s">
-        <v>31</v>
+        <v>86</v>
       </c>
       <c r="H49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J49">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="K49" t="s">
+        <v>89</v>
       </c>
       <c r="L49">
         <v>7</v>
@@ -3822,32 +3894,27 @@
       <c r="Y49">
         <v>0</v>
       </c>
-      <c r="Z49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA49" s="2"/>
+    </row>
+    <row r="50" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="B50" t="s">
-        <v>45</v>
-      </c>
-      <c r="C50" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D50" t="str">
         <f t="shared" si="1"/>
-        <v>RAS27_Demi</v>
+        <v>RAS28</v>
       </c>
       <c r="E50" s="1">
-        <v>44939</v>
+        <v>44974</v>
       </c>
       <c r="F50" s="1">
-        <v>44944</v>
+        <v>44979</v>
       </c>
       <c r="G50" t="s">
-        <v>31</v>
+        <v>86</v>
       </c>
       <c r="H50">
         <v>1</v>
@@ -3856,13 +3923,16 @@
         <v>0</v>
       </c>
       <c r="J50">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="K50" t="s">
+        <v>89</v>
       </c>
       <c r="L50">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="M50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N50">
         <v>3</v>
@@ -3880,7 +3950,7 @@
         <v>1</v>
       </c>
       <c r="V50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W50">
         <v>0</v>
@@ -3894,20 +3964,23 @@
       <c r="Z50">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA50" s="2">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="51" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>96</v>
       </c>
       <c r="B51" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C51" t="s">
         <v>90</v>
       </c>
       <c r="D51" t="str">
         <f t="shared" si="1"/>
-        <v>OPT0419_Demi</v>
+        <v>RAS05_Demi</v>
       </c>
       <c r="E51" s="1">
         <v>44988</v>
@@ -3919,16 +3992,16 @@
         <v>86</v>
       </c>
       <c r="H51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J51">
         <v>3</v>
       </c>
       <c r="L51">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M51">
         <v>0</v>
@@ -3949,7 +4022,7 @@
         <v>1</v>
       </c>
       <c r="V51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W51">
         <v>0</v>
@@ -3960,20 +4033,26 @@
       <c r="Y51">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="Z51">
+        <v>0</v>
+      </c>
+      <c r="AA51" s="2">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="52" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>96</v>
       </c>
       <c r="B52" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="C52" t="s">
         <v>90</v>
       </c>
       <c r="D52" t="str">
         <f t="shared" si="1"/>
-        <v>RAS05_Demi</v>
+        <v>RAS16_Demi</v>
       </c>
       <c r="E52" s="1">
         <v>44988</v>
@@ -3994,7 +4073,7 @@
         <v>3</v>
       </c>
       <c r="L52">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="M52">
         <v>0</v>
@@ -4015,7 +4094,7 @@
         <v>1</v>
       </c>
       <c r="V52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W52">
         <v>0</v>
@@ -4029,20 +4108,23 @@
       <c r="Z52">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA52" s="2">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="53" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>96</v>
       </c>
       <c r="B53" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C53" t="s">
         <v>90</v>
       </c>
       <c r="D53" t="str">
         <f t="shared" si="1"/>
-        <v>RAS16_Demi</v>
+        <v>RAS22_Demi</v>
       </c>
       <c r="E53" s="1">
         <v>44988</v>
@@ -4063,7 +4145,7 @@
         <v>3</v>
       </c>
       <c r="L53">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="M53">
         <v>0</v>
@@ -4084,7 +4166,7 @@
         <v>1</v>
       </c>
       <c r="V53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W53">
         <v>0</v>
@@ -4096,22 +4178,25 @@
         <v>0</v>
       </c>
       <c r="Z53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="AA53" s="2">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="54" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>96</v>
       </c>
       <c r="B54" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C54" t="s">
         <v>90</v>
       </c>
       <c r="D54" t="str">
         <f t="shared" si="1"/>
-        <v>RAS22_Demi</v>
+        <v>RAS24_Demi</v>
       </c>
       <c r="E54" s="1">
         <v>44988</v>
@@ -4132,16 +4217,16 @@
         <v>3</v>
       </c>
       <c r="L54">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="M54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N54">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O54" t="s">
-        <v>21</v>
+        <v>97</v>
       </c>
       <c r="Q54">
         <v>0</v>
@@ -4150,7 +4235,7 @@
         <v>1</v>
       </c>
       <c r="U54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V54">
         <v>0</v>
@@ -4159,28 +4244,31 @@
         <v>0</v>
       </c>
       <c r="X54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z54">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA54" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>96</v>
       </c>
       <c r="B55" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="C55" t="s">
         <v>90</v>
       </c>
       <c r="D55" t="str">
-        <f t="shared" ref="D55" si="2">IF(NOT(ISBLANK(C55)),B55&amp;"_"&amp;C55,B55)</f>
-        <v>RAS24_Demi</v>
+        <f t="shared" si="1"/>
+        <v>OPT0419_Demi</v>
       </c>
       <c r="E55" s="1">
         <v>44988</v>
@@ -4192,25 +4280,25 @@
         <v>86</v>
       </c>
       <c r="H55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J55">
         <v>3</v>
       </c>
       <c r="L55">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="M55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N55">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O55" t="s">
-        <v>97</v>
+        <v>21</v>
       </c>
       <c r="Q55">
         <v>0</v>
@@ -4219,7 +4307,7 @@
         <v>1</v>
       </c>
       <c r="U55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V55">
         <v>0</v>
@@ -4228,23 +4316,23 @@
         <v>0</v>
       </c>
       <c r="X55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z55">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="AA55" s="2"/>
+    </row>
+    <row r="56" spans="1:27" x14ac:dyDescent="0.2">
       <c r="E56" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:Y55" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Y50">
-      <sortCondition ref="A2:A50"/>
-      <sortCondition ref="D2:D50"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Y55">
+      <sortCondition ref="E1:E55"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adjusted code to analyse AUC and to aggregate by variables
</commit_message>
<xml_diff>
--- a/resources/Screening_overview.xlsx
+++ b/resources/Screening_overview.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mhuismans/surfdrive/Promotie/12. STRATEGIC/Analyse 2.0/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SURFdrive\Lsmabers\Shared\12. Early Metastatic vs Late Stage\Analyse 2.0\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD32BCE4-A185-7E4D-915D-11C510436C35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="16020"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet 1'!$A$1:$Y$55</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -347,7 +346,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy/mm/dd\ hh:mm:ss"/>
   </numFmts>
@@ -685,29 +684,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AA54" sqref="AA54"/>
+      <selection pane="bottomRight" activeCell="W13" sqref="W13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.33203125" customWidth="1"/>
-    <col min="11" max="11" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="64.5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" customWidth="1"/>
+    <col min="11" max="11" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="64.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -790,7 +789,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -838,7 +837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -886,7 +885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -943,7 +942,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -991,7 +990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -1048,7 +1047,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -1105,7 +1104,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -1171,7 +1170,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -1235,7 +1234,7 @@
       </c>
       <c r="AA9" s="2"/>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -1295,7 +1294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -1355,7 +1354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -1406,7 +1405,7 @@
         <v>1</v>
       </c>
       <c r="W12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X12">
         <v>0</v>
@@ -1421,7 +1420,7 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -1472,7 +1471,7 @@
         <v>0</v>
       </c>
       <c r="W13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X13">
         <v>0</v>
@@ -1481,7 +1480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -1547,7 +1546,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -1613,7 +1612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -1676,7 +1675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -1745,7 +1744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>43</v>
       </c>
@@ -1814,7 +1813,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -1886,7 +1885,7 @@
         <v>0.37</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>49</v>
       </c>
@@ -1961,7 +1960,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>49</v>
       </c>
@@ -2031,7 +2030,7 @@
       </c>
       <c r="AA21" s="2"/>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>54</v>
       </c>
@@ -2103,7 +2102,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>54</v>
       </c>
@@ -2175,7 +2174,7 @@
         <v>0.39</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>54</v>
       </c>
@@ -2242,7 +2241,7 @@
       </c>
       <c r="AA24" s="2"/>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>59</v>
       </c>
@@ -2317,7 +2316,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>59</v>
       </c>
@@ -2387,7 +2386,7 @@
       </c>
       <c r="AA26" s="2"/>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>64</v>
       </c>
@@ -2462,7 +2461,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>64</v>
       </c>
@@ -2532,7 +2531,7 @@
       </c>
       <c r="AA28" s="2"/>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>64</v>
       </c>
@@ -2607,7 +2606,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>64</v>
       </c>
@@ -2682,7 +2681,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>70</v>
       </c>
@@ -2748,7 +2747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>70</v>
       </c>
@@ -2814,7 +2813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>70</v>
       </c>
@@ -2880,7 +2879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>82</v>
       </c>
@@ -2888,7 +2887,7 @@
         <v>75</v>
       </c>
       <c r="D34" t="str">
-        <f t="shared" ref="D34:D65" si="1">IF(NOT(ISBLANK(C34)),B34&amp;"_"&amp;C34,B34)</f>
+        <f t="shared" ref="D34:D55" si="1">IF(NOT(ISBLANK(C34)),B34&amp;"_"&amp;C34,B34)</f>
         <v>OPT0039</v>
       </c>
       <c r="E34" s="1">
@@ -2937,7 +2936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>82</v>
       </c>
@@ -2997,7 +2996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>82</v>
       </c>
@@ -3060,7 +3059,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>82</v>
       </c>
@@ -3123,7 +3122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>83</v>
       </c>
@@ -3183,7 +3182,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>83</v>
       </c>
@@ -3246,7 +3245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>83</v>
       </c>
@@ -3309,7 +3308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>83</v>
       </c>
@@ -3366,7 +3365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>83</v>
       </c>
@@ -3426,7 +3425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>83</v>
       </c>
@@ -3486,7 +3485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>95</v>
       </c>
@@ -3558,7 +3557,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="45" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>95</v>
       </c>
@@ -3624,7 +3623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>95</v>
       </c>
@@ -3691,7 +3690,7 @@
       </c>
       <c r="AA46" s="2"/>
     </row>
-    <row r="47" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>95</v>
       </c>
@@ -3763,7 +3762,7 @@
         <v>0.37</v>
       </c>
     </row>
-    <row r="48" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>85</v>
       </c>
@@ -3829,7 +3828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>85</v>
       </c>
@@ -3896,7 +3895,7 @@
       </c>
       <c r="AA49" s="2"/>
     </row>
-    <row r="50" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>85</v>
       </c>
@@ -3968,7 +3967,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="51" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>96</v>
       </c>
@@ -4040,7 +4039,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="52" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>96</v>
       </c>
@@ -4112,7 +4111,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="53" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>96</v>
       </c>
@@ -4184,7 +4183,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="54" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>96</v>
       </c>
@@ -4256,7 +4255,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>96</v>
       </c>
@@ -4326,12 +4325,12 @@
       </c>
       <c r="AA55" s="2"/>
     </row>
-    <row r="56" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:27" x14ac:dyDescent="0.25">
       <c r="E56" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Y55" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Y55">
+  <autoFilter ref="A1:Y55">
+    <sortState ref="A2:Y55">
       <sortCondition ref="E1:E55"/>
     </sortState>
   </autoFilter>

</xml_diff>